<commit_message>
Removed slicing of top 5 configurations
</commit_message>
<xml_diff>
--- a/interconnection_testing.xlsx
+++ b/interconnection_testing.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="152">
   <si>
     <t>-00011110+</t>
   </si>
@@ -52,16 +52,427 @@
     <t>-1001+-0011+</t>
   </si>
   <si>
-    <t>-1001+-1100+</t>
-  </si>
-  <si>
     <t>-0110+-0011+</t>
   </si>
   <si>
-    <t>-1100+-1001+</t>
+    <t>-0011+-1001+</t>
   </si>
   <si>
-    <t>-1100+-0110+</t>
+    <t>-+-(0110)0011+</t>
+  </si>
+  <si>
+    <t>-00(1001)11+</t>
+  </si>
+  <si>
+    <t>-11(0110)00+</t>
+  </si>
+  <si>
+    <t>-11(1001)00+</t>
+  </si>
+  <si>
+    <t>-00(0110)11+</t>
+  </si>
+  <si>
+    <t>-+-11(0110)00+</t>
+  </si>
+  <si>
+    <t>-0011(1001)+-+</t>
+  </si>
+  <si>
+    <t>-11(0110)00+-+</t>
+  </si>
+  <si>
+    <t>-11(0110)+-00+</t>
+  </si>
+  <si>
+    <t>-00(1001)+-11+</t>
+  </si>
+  <si>
+    <t>-00(0110)+-11+</t>
+  </si>
+  <si>
+    <t>-11(1001)+-00+</t>
+  </si>
+  <si>
+    <t>-11+-(1001)00+</t>
+  </si>
+  <si>
+    <t>-+-10010011+</t>
+  </si>
+  <si>
+    <t>-+-11000110+</t>
+  </si>
+  <si>
+    <t>-10010011+</t>
+  </si>
+  <si>
+    <t>-10011100+</t>
+  </si>
+  <si>
+    <t>-+-10011100+</t>
+  </si>
+  <si>
+    <t>-01101100+</t>
+  </si>
+  <si>
+    <t>-01100011+</t>
+  </si>
+  <si>
+    <t>-00111001+</t>
+  </si>
+  <si>
+    <t>-11000110+</t>
+  </si>
+  <si>
+    <t>-11001001+</t>
+  </si>
+  <si>
+    <t>-00110110+</t>
+  </si>
+  <si>
+    <t>-00011011+</t>
+  </si>
+  <si>
+    <t>-10000111+</t>
+  </si>
+  <si>
+    <t>-10110001+</t>
+  </si>
+  <si>
+    <t>-00100111+</t>
+  </si>
+  <si>
+    <t>-01110010+</t>
+  </si>
+  <si>
+    <t>-+-11010010+</t>
+  </si>
+  <si>
+    <t>-+-11100100+</t>
+  </si>
+  <si>
+    <t>-+-11100001+</t>
+  </si>
+  <si>
+    <t>-10110100+</t>
+  </si>
+  <si>
+    <t>-+-01001110+</t>
+  </si>
+  <si>
+    <t>-00101101+</t>
+  </si>
+  <si>
+    <t>-+-01110010+</t>
+  </si>
+  <si>
+    <t>-11100001+</t>
+  </si>
+  <si>
+    <t>-11010010+</t>
+  </si>
+  <si>
+    <t>-01111000+</t>
+  </si>
+  <si>
+    <t>-10001101+</t>
+  </si>
+  <si>
+    <t>-+-00011011+</t>
+  </si>
+  <si>
+    <t>-+-10001101+</t>
+  </si>
+  <si>
+    <t>-11100100+</t>
+  </si>
+  <si>
+    <t>-11011000+</t>
+  </si>
+  <si>
+    <t>-01001011+</t>
+  </si>
+  <si>
+    <t>-01001110+</t>
+  </si>
+  <si>
+    <t>-10011100+-+</t>
+  </si>
+  <si>
+    <t>-01101100+-+</t>
+  </si>
+  <si>
+    <t>-01100011+-+</t>
+  </si>
+  <si>
+    <t>-11100100+-+</t>
+  </si>
+  <si>
+    <t>-00101101+-+</t>
+  </si>
+  <si>
+    <t>-11010010+-+</t>
+  </si>
+  <si>
+    <t>-11100001+-+</t>
+  </si>
+  <si>
+    <t>-0111+-0010+</t>
+  </si>
+  <si>
+    <t>-0100+-1110+</t>
+  </si>
+  <si>
+    <t>-1110+-0100+</t>
+  </si>
+  <si>
+    <t>-0010+-1101+</t>
+  </si>
+  <si>
+    <t>-1101+-0010+</t>
+  </si>
+  <si>
+    <t>-00(1101)+-10+</t>
+  </si>
+  <si>
+    <t>-11(0001)+-10+</t>
+  </si>
+  <si>
+    <t>-00(1011)+-01+</t>
+  </si>
+  <si>
+    <t>-10(1101)+-00+</t>
+  </si>
+  <si>
+    <t>-10(0001)+-11+</t>
+  </si>
+  <si>
+    <t>-01(0010)+-11+</t>
+  </si>
+  <si>
+    <t>-01(1011)+-00+</t>
+  </si>
+  <si>
+    <t>-100100+-11+</t>
+  </si>
+  <si>
+    <t>-011000+-11+</t>
+  </si>
+  <si>
+    <t>-11+-(0100)10+</t>
+  </si>
+  <si>
+    <t>-00+-(1110)01+</t>
+  </si>
+  <si>
+    <t>-11+-(1000)01+</t>
+  </si>
+  <si>
+    <t>-11+-011000+</t>
+  </si>
+  <si>
+    <t>-11+-000110+</t>
+  </si>
+  <si>
+    <t>-00+-111001+</t>
+  </si>
+  <si>
+    <t>-11+-100100+</t>
+  </si>
+  <si>
+    <t>-00+-100111+</t>
+  </si>
+  <si>
+    <t>-00+-110110+</t>
+  </si>
+  <si>
+    <t>-00+-011110+</t>
+  </si>
+  <si>
+    <t>-11+-100001+</t>
+  </si>
+  <si>
+    <t>-11+-010010+</t>
+  </si>
+  <si>
+    <t>-10(1101)00+</t>
+  </si>
+  <si>
+    <t>-01(0010)11+</t>
+  </si>
+  <si>
+    <t>-10(0100)11+</t>
+  </si>
+  <si>
+    <t>-10(0001)11+</t>
+  </si>
+  <si>
+    <t>-01(1011)00+</t>
+  </si>
+  <si>
+    <t>-01(1000)11+</t>
+  </si>
+  <si>
+    <t>-01(1110)00+</t>
+  </si>
+  <si>
+    <t>-10(0111)00+</t>
+  </si>
+  <si>
+    <t>-00(1110)01+</t>
+  </si>
+  <si>
+    <t>-+-(1110)0001+</t>
+  </si>
+  <si>
+    <t>-+-01(1110)00+</t>
+  </si>
+  <si>
+    <t>-11(0001)10+</t>
+  </si>
+  <si>
+    <t>-+-01(1011)00+</t>
+  </si>
+  <si>
+    <t>-+-(0100)1011+</t>
+  </si>
+  <si>
+    <t>-11(0010)01+</t>
+  </si>
+  <si>
+    <t>-+-11(0001)10+</t>
+  </si>
+  <si>
+    <t>-+-(0010)0111+</t>
+  </si>
+  <si>
+    <t>-+-(0111)1000+</t>
+  </si>
+  <si>
+    <t>-+-(1011)0001+</t>
+  </si>
+  <si>
+    <t>-+-10(0001)11+</t>
+  </si>
+  <si>
+    <t>-00(1101)10+</t>
+  </si>
+  <si>
+    <t>-+-(1101)1000+</t>
+  </si>
+  <si>
+    <t>-+-(0001)1110+</t>
+  </si>
+  <si>
+    <t>-11(0100)10+</t>
+  </si>
+  <si>
+    <t>-00(1011)01+</t>
+  </si>
+  <si>
+    <t>-11(1000)01+</t>
+  </si>
+  <si>
+    <t>-0100(1011)+-+</t>
+  </si>
+  <si>
+    <t>-01(1011)00+-+</t>
+  </si>
+  <si>
+    <t>-10(0100)11+-+</t>
+  </si>
+  <si>
+    <t>-11(0001)10+-+</t>
+  </si>
+  <si>
+    <t>-1011(0001)+-+</t>
+  </si>
+  <si>
+    <t>-11(0100)10+-+</t>
+  </si>
+  <si>
+    <t>-1000(1101)+-+</t>
+  </si>
+  <si>
+    <t>-1000(0111)+-+</t>
+  </si>
+  <si>
+    <t>-00(1110)01+-+</t>
+  </si>
+  <si>
+    <t>-10(1101)00+-+</t>
+  </si>
+  <si>
+    <t>-01(1110)00+-+</t>
+  </si>
+  <si>
+    <t>-0010(0111)+-+</t>
+  </si>
+  <si>
+    <t>-10(0011)01+</t>
+  </si>
+  <si>
+    <t>-10(1100)01+</t>
+  </si>
+  <si>
+    <t>-01(1100)10+</t>
+  </si>
+  <si>
+    <t>-01(0011)10+</t>
+  </si>
+  <si>
+    <t>-+-01(1100)10+</t>
+  </si>
+  <si>
+    <t>-1001(0011)+-+</t>
+  </si>
+  <si>
+    <t>-1001(1100)+-+</t>
+  </si>
+  <si>
+    <t>-10(0011)01+-+</t>
+  </si>
+  <si>
+    <t>-01(0011)10+-+</t>
+  </si>
+  <si>
+    <t>-010011+-10+</t>
+  </si>
+  <si>
+    <t>-001101+-10+</t>
+  </si>
+  <si>
+    <t>-001011+-01+</t>
+  </si>
+  <si>
+    <t>-000111+-10+</t>
+  </si>
+  <si>
+    <t>-110001+-10+</t>
+  </si>
+  <si>
+    <t>-111000+-01+</t>
+  </si>
+  <si>
+    <t>-110010+-01+</t>
+  </si>
+  <si>
+    <t>-01(0011)+-10+</t>
+  </si>
+  <si>
+    <t>-01+-001011+</t>
+  </si>
+  <si>
+    <t>-01+-110010+</t>
+  </si>
+  <si>
+    <t>-10+-110001+</t>
+  </si>
+  <si>
+    <t>-10+-000111+</t>
+  </si>
+  <si>
+    <t>-01+-(0011)10+</t>
   </si>
 </sst>
 </file>
@@ -35644,13 +36055,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:EO4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:145">
       <c r="B1" s="1" t="s">
         <v>10</v>
       </c>
@@ -35666,8 +36077,425 @@
       <c r="F1" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="BI1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="BK1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="BL1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BM1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="BN1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="BO1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BP1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="BQ1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="BR1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="BS1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BT1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="BU1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="BV1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="BW1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="BX1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="BY1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="BZ1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="CA1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="CB1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="CC1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="CD1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="CE1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="CF1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="CG1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="CH1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="CI1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="CJ1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="CK1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="CL1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="CM1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="CN1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="CO1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="CP1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="CQ1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="CR1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="CS1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="CT1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="CU1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="CV1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="CW1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="CX1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="CY1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="CZ1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="DA1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="DB1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="DC1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="DD1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="DE1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="DF1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="DG1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="DH1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="DI1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="DJ1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="DK1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="DL1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="DM1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="DN1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="DO1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="DP1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="DQ1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="DR1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="DS1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="DT1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="DU1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="DV1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="DW1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="DX1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="DY1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="DZ1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="EA1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="EB1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="EC1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="ED1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="EE1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="EF1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="EG1" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="EH1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="EI1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="EJ1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="EK1" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="EL1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="EM1" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="EN1" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="EO1" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" spans="1:145">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -35678,16 +36506,433 @@
         <v>8.801120388643609</v>
       </c>
       <c r="D2">
-        <v>8.801120388643609</v>
+        <v>8.788755512621808</v>
       </c>
       <c r="E2">
-        <v>8.788755512621808</v>
+        <v>8.001250091340133</v>
       </c>
       <c r="F2">
-        <v>8.788755512621808</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>8.001250091338749</v>
+      </c>
+      <c r="G2">
+        <v>8.001250091338749</v>
+      </c>
+      <c r="H2">
+        <v>8.001250091338749</v>
+      </c>
+      <c r="I2">
+        <v>8.001250091338749</v>
+      </c>
+      <c r="J2">
+        <v>8.001250091338287</v>
+      </c>
+      <c r="K2">
+        <v>7.984416186743372</v>
+      </c>
+      <c r="L2">
+        <v>7.98441618674291</v>
+      </c>
+      <c r="M2">
+        <v>5.861708947088221</v>
+      </c>
+      <c r="N2">
+        <v>5.861708947088221</v>
+      </c>
+      <c r="O2">
+        <v>5.861708947088221</v>
+      </c>
+      <c r="P2">
+        <v>5.861708947088221</v>
+      </c>
+      <c r="Q2">
+        <v>5.822102573298681</v>
+      </c>
+      <c r="R2">
+        <v>5.332393298878278</v>
+      </c>
+      <c r="S2">
+        <v>5.332393298878278</v>
+      </c>
+      <c r="T2">
+        <v>5.332393298878278</v>
+      </c>
+      <c r="U2">
+        <v>5.332393298878278</v>
+      </c>
+      <c r="V2">
+        <v>5.332393298878278</v>
+      </c>
+      <c r="W2">
+        <v>5.332393298878278</v>
+      </c>
+      <c r="X2">
+        <v>5.332393298878278</v>
+      </c>
+      <c r="Y2">
+        <v>5.332393298877041</v>
+      </c>
+      <c r="Z2">
+        <v>5.332393298877041</v>
+      </c>
+      <c r="AA2">
+        <v>5.332393298877041</v>
+      </c>
+      <c r="AB2">
+        <v>5.332393298877041</v>
+      </c>
+      <c r="AC2">
+        <v>5.332393298875804</v>
+      </c>
+      <c r="AD2">
+        <v>5.332393298875804</v>
+      </c>
+      <c r="AE2">
+        <v>5.332393298875804</v>
+      </c>
+      <c r="AF2">
+        <v>5.332393298875804</v>
+      </c>
+      <c r="AG2">
+        <v>5.332393298875804</v>
+      </c>
+      <c r="AH2">
+        <v>5.332393298875804</v>
+      </c>
+      <c r="AI2">
+        <v>5.332393298875804</v>
+      </c>
+      <c r="AJ2">
+        <v>5.332393298875804</v>
+      </c>
+      <c r="AK2">
+        <v>5.332393298875804</v>
+      </c>
+      <c r="AL2">
+        <v>5.332393298875804</v>
+      </c>
+      <c r="AM2">
+        <v>5.332393298875804</v>
+      </c>
+      <c r="AN2">
+        <v>5.332393298875804</v>
+      </c>
+      <c r="AO2">
+        <v>5.332393298875804</v>
+      </c>
+      <c r="AP2">
+        <v>5.332393298875804</v>
+      </c>
+      <c r="AQ2">
+        <v>5.332393298875804</v>
+      </c>
+      <c r="AR2">
+        <v>5.332393298875804</v>
+      </c>
+      <c r="AS2">
+        <v>5.332393298875804</v>
+      </c>
+      <c r="AT2">
+        <v>5.332393298875804</v>
+      </c>
+      <c r="AU2">
+        <v>5.332393298875804</v>
+      </c>
+      <c r="AV2">
+        <v>5.332393298875804</v>
+      </c>
+      <c r="AW2">
+        <v>5.332393298875804</v>
+      </c>
+      <c r="AX2">
+        <v>5.332393298875804</v>
+      </c>
+      <c r="AY2">
+        <v>5.332393298875804</v>
+      </c>
+      <c r="AZ2">
+        <v>5.328386870950171</v>
+      </c>
+      <c r="BA2">
+        <v>5.328386870950171</v>
+      </c>
+      <c r="BB2">
+        <v>5.328386870950171</v>
+      </c>
+      <c r="BC2">
+        <v>5.328386870948934</v>
+      </c>
+      <c r="BD2">
+        <v>5.328386870947697</v>
+      </c>
+      <c r="BE2">
+        <v>5.328386870947697</v>
+      </c>
+      <c r="BF2">
+        <v>5.328386870947697</v>
+      </c>
+      <c r="BG2">
+        <v>5.328316008944133</v>
+      </c>
+      <c r="BH2">
+        <v>5.328316008944133</v>
+      </c>
+      <c r="BI2">
+        <v>5.328316008943515</v>
+      </c>
+      <c r="BJ2">
+        <v>5.328316008943515</v>
+      </c>
+      <c r="BK2">
+        <v>5.328316008943515</v>
+      </c>
+      <c r="BL2">
+        <v>4.534951375588803</v>
+      </c>
+      <c r="BM2">
+        <v>4.534951375588803</v>
+      </c>
+      <c r="BN2">
+        <v>4.534951375588803</v>
+      </c>
+      <c r="BO2">
+        <v>4.516146415032845</v>
+      </c>
+      <c r="BP2">
+        <v>4.516146415032845</v>
+      </c>
+      <c r="BQ2">
+        <v>4.516146415032845</v>
+      </c>
+      <c r="BR2">
+        <v>4.51614641503254</v>
+      </c>
+      <c r="BS2">
+        <v>4.516144520055231</v>
+      </c>
+      <c r="BT2">
+        <v>4.516144520055231</v>
+      </c>
+      <c r="BU2">
+        <v>4.482102099013621</v>
+      </c>
+      <c r="BV2">
+        <v>4.482102099013621</v>
+      </c>
+      <c r="BW2">
+        <v>4.482102099013621</v>
+      </c>
+      <c r="BX2">
+        <v>4.482100137025595</v>
+      </c>
+      <c r="BY2">
+        <v>4.482100137025595</v>
+      </c>
+      <c r="BZ2">
+        <v>4.482100137025595</v>
+      </c>
+      <c r="CA2">
+        <v>4.482100137025595</v>
+      </c>
+      <c r="CB2">
+        <v>4.482100137025595</v>
+      </c>
+      <c r="CC2">
+        <v>4.482100137025595</v>
+      </c>
+      <c r="CD2">
+        <v>4.482100137025443</v>
+      </c>
+      <c r="CE2">
+        <v>4.482100137025443</v>
+      </c>
+      <c r="CF2">
+        <v>4.482100137025443</v>
+      </c>
+      <c r="CG2">
+        <v>4.10818043817293</v>
+      </c>
+      <c r="CH2">
+        <v>4.10818043817293</v>
+      </c>
+      <c r="CI2">
+        <v>4.10818043817293</v>
+      </c>
+      <c r="CJ2">
+        <v>4.10818043817293</v>
+      </c>
+      <c r="CK2">
+        <v>4.10818043817293</v>
+      </c>
+      <c r="CL2">
+        <v>4.10818043817293</v>
+      </c>
+      <c r="CM2">
+        <v>4.10818043817293</v>
+      </c>
+      <c r="CN2">
+        <v>4.10818043817293</v>
+      </c>
+      <c r="CO2">
+        <v>4.108180438171984</v>
+      </c>
+      <c r="CP2">
+        <v>4.108180438171984</v>
+      </c>
+      <c r="CQ2">
+        <v>4.108180438171984</v>
+      </c>
+      <c r="CR2">
+        <v>4.108180438171984</v>
+      </c>
+      <c r="CS2">
+        <v>4.108180438171984</v>
+      </c>
+      <c r="CT2">
+        <v>4.108180438171984</v>
+      </c>
+      <c r="CU2">
+        <v>4.108180438171984</v>
+      </c>
+      <c r="CV2">
+        <v>4.108180438171984</v>
+      </c>
+      <c r="CW2">
+        <v>4.108180438171984</v>
+      </c>
+      <c r="CX2">
+        <v>4.108180438171984</v>
+      </c>
+      <c r="CY2">
+        <v>4.108180438171984</v>
+      </c>
+      <c r="CZ2">
+        <v>4.108180438171984</v>
+      </c>
+      <c r="DA2">
+        <v>4.108180438171984</v>
+      </c>
+      <c r="DB2">
+        <v>4.108180438171984</v>
+      </c>
+      <c r="DC2">
+        <v>4.108180438171984</v>
+      </c>
+      <c r="DD2">
+        <v>4.108180438171038</v>
+      </c>
+      <c r="DE2">
+        <v>4.108180438171038</v>
+      </c>
+      <c r="DF2">
+        <v>4.108180438171038</v>
+      </c>
+      <c r="DG2">
+        <v>4.108180438171038</v>
+      </c>
+      <c r="DH2">
+        <v>4.104247074435842</v>
+      </c>
+      <c r="DI2">
+        <v>4.104247074435842</v>
+      </c>
+      <c r="DJ2">
+        <v>4.104247074435842</v>
+      </c>
+      <c r="DK2">
+        <v>4.104247074435842</v>
+      </c>
+      <c r="DL2">
+        <v>4.104247074435842</v>
+      </c>
+      <c r="DM2">
+        <v>4.104247074435842</v>
+      </c>
+      <c r="DN2">
+        <v>4.104247074435842</v>
+      </c>
+      <c r="DO2">
+        <v>4.104247074435842</v>
+      </c>
+      <c r="DP2">
+        <v>4.104247074435842</v>
+      </c>
+      <c r="DQ2">
+        <v>4.104247074434896</v>
+      </c>
+      <c r="DR2">
+        <v>4.104247074434896</v>
+      </c>
+      <c r="DS2">
+        <v>4.104247074433951</v>
+      </c>
+      <c r="DT2">
+        <v>3.907866429488499</v>
+      </c>
+      <c r="DU2">
+        <v>3.907866429488499</v>
+      </c>
+      <c r="DV2">
+        <v>3.907866429488499</v>
+      </c>
+      <c r="DW2">
+        <v>3.907866429488499</v>
+      </c>
+      <c r="DX2">
+        <v>3.907866429487128</v>
+      </c>
+      <c r="DY2">
+        <v>3.904178273638084</v>
+      </c>
+      <c r="DZ2">
+        <v>3.904178273638084</v>
+      </c>
+      <c r="EA2">
+        <v>3.904178273637174</v>
+      </c>
+      <c r="EB2">
+        <v>3.904178273637174</v>
+      </c>
+      <c r="EC2">
+        <v>2.535796439376919</v>
+      </c>
+      <c r="ED2">
+        <v>2.535796439376919</v>
+      </c>
+      <c r="EE2">
+        <v>2.535796439376919</v>
+      </c>
+      <c r="EF2">
+        <v>2.535796439376919</v>
+      </c>
+      <c r="EG2">
+        <v>2.535796439376919</v>
+      </c>
+      <c r="EH2">
+        <v>2.535796439376919</v>
+      </c>
+      <c r="EI2">
+        <v>2.535796439376919</v>
+      </c>
+      <c r="EJ2">
+        <v>2.535748417970078</v>
+      </c>
+      <c r="EK2">
+        <v>2.5282469173021</v>
+      </c>
+      <c r="EL2">
+        <v>2.5282469173021</v>
+      </c>
+      <c r="EM2">
+        <v>2.5282469173021</v>
+      </c>
+      <c r="EN2">
+        <v>2.5282469173021</v>
+      </c>
+      <c r="EO2">
+        <v>2.52819889594343</v>
+      </c>
+    </row>
+    <row r="3" spans="1:145">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -35701,13 +36946,430 @@
         <v>1.310000000000001</v>
       </c>
       <c r="E3">
-        <v>1.310000000000001</v>
+        <v>2.030000000000001</v>
       </c>
       <c r="F3">
-        <v>1.310000000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>2.030000000000001</v>
+      </c>
+      <c r="G3">
+        <v>2.030000000000001</v>
+      </c>
+      <c r="H3">
+        <v>2.030000000000001</v>
+      </c>
+      <c r="I3">
+        <v>2.030000000000001</v>
+      </c>
+      <c r="J3">
+        <v>2.030000000000001</v>
+      </c>
+      <c r="K3">
+        <v>2.030000000000001</v>
+      </c>
+      <c r="L3">
+        <v>2.030000000000001</v>
+      </c>
+      <c r="M3">
+        <v>0.6800000000000004</v>
+      </c>
+      <c r="N3">
+        <v>0.6800000000000004</v>
+      </c>
+      <c r="O3">
+        <v>0.6800000000000004</v>
+      </c>
+      <c r="P3">
+        <v>0.6800000000000004</v>
+      </c>
+      <c r="Q3">
+        <v>0.6700000000000004</v>
+      </c>
+      <c r="R3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="S3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="T3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="U3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="V3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="W3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="X3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="Y3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="Z3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="AA3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="AB3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="AC3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="AD3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="AE3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="AF3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="AG3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="AH3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="AI3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="AJ3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="AK3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="AL3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="AM3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="AN3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="AO3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="AP3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="AQ3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="AR3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="AS3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="AT3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="AU3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="AV3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="AW3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="AX3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="AY3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="AZ3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="BA3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="BB3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="BC3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="BD3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="BE3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="BF3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="BG3">
+        <v>1.360000000000001</v>
+      </c>
+      <c r="BH3">
+        <v>1.360000000000001</v>
+      </c>
+      <c r="BI3">
+        <v>1.360000000000001</v>
+      </c>
+      <c r="BJ3">
+        <v>1.360000000000001</v>
+      </c>
+      <c r="BK3">
+        <v>1.360000000000001</v>
+      </c>
+      <c r="BL3">
+        <v>0.6700000000000004</v>
+      </c>
+      <c r="BM3">
+        <v>0.6700000000000004</v>
+      </c>
+      <c r="BN3">
+        <v>0.6700000000000004</v>
+      </c>
+      <c r="BO3">
+        <v>0.6700000000000004</v>
+      </c>
+      <c r="BP3">
+        <v>0.6700000000000004</v>
+      </c>
+      <c r="BQ3">
+        <v>0.6700000000000004</v>
+      </c>
+      <c r="BR3">
+        <v>0.6700000000000004</v>
+      </c>
+      <c r="BS3">
+        <v>0.6700000000000004</v>
+      </c>
+      <c r="BT3">
+        <v>0.6700000000000004</v>
+      </c>
+      <c r="BU3">
+        <v>0.6700000000000004</v>
+      </c>
+      <c r="BV3">
+        <v>0.6700000000000004</v>
+      </c>
+      <c r="BW3">
+        <v>0.6700000000000004</v>
+      </c>
+      <c r="BX3">
+        <v>0.6700000000000004</v>
+      </c>
+      <c r="BY3">
+        <v>0.6700000000000004</v>
+      </c>
+      <c r="BZ3">
+        <v>0.6700000000000004</v>
+      </c>
+      <c r="CA3">
+        <v>0.6700000000000004</v>
+      </c>
+      <c r="CB3">
+        <v>0.6700000000000004</v>
+      </c>
+      <c r="CC3">
+        <v>0.6700000000000004</v>
+      </c>
+      <c r="CD3">
+        <v>0.6700000000000004</v>
+      </c>
+      <c r="CE3">
+        <v>0.6700000000000004</v>
+      </c>
+      <c r="CF3">
+        <v>0.6700000000000004</v>
+      </c>
+      <c r="CG3">
+        <v>2.08</v>
+      </c>
+      <c r="CH3">
+        <v>2.08</v>
+      </c>
+      <c r="CI3">
+        <v>2.08</v>
+      </c>
+      <c r="CJ3">
+        <v>2.08</v>
+      </c>
+      <c r="CK3">
+        <v>2.08</v>
+      </c>
+      <c r="CL3">
+        <v>2.08</v>
+      </c>
+      <c r="CM3">
+        <v>2.08</v>
+      </c>
+      <c r="CN3">
+        <v>2.08</v>
+      </c>
+      <c r="CO3">
+        <v>2.08</v>
+      </c>
+      <c r="CP3">
+        <v>2.08</v>
+      </c>
+      <c r="CQ3">
+        <v>2.08</v>
+      </c>
+      <c r="CR3">
+        <v>2.08</v>
+      </c>
+      <c r="CS3">
+        <v>2.08</v>
+      </c>
+      <c r="CT3">
+        <v>2.08</v>
+      </c>
+      <c r="CU3">
+        <v>2.08</v>
+      </c>
+      <c r="CV3">
+        <v>2.08</v>
+      </c>
+      <c r="CW3">
+        <v>2.08</v>
+      </c>
+      <c r="CX3">
+        <v>2.08</v>
+      </c>
+      <c r="CY3">
+        <v>2.08</v>
+      </c>
+      <c r="CZ3">
+        <v>2.08</v>
+      </c>
+      <c r="DA3">
+        <v>2.08</v>
+      </c>
+      <c r="DB3">
+        <v>2.08</v>
+      </c>
+      <c r="DC3">
+        <v>2.08</v>
+      </c>
+      <c r="DD3">
+        <v>2.08</v>
+      </c>
+      <c r="DE3">
+        <v>2.08</v>
+      </c>
+      <c r="DF3">
+        <v>2.08</v>
+      </c>
+      <c r="DG3">
+        <v>2.08</v>
+      </c>
+      <c r="DH3">
+        <v>2.08</v>
+      </c>
+      <c r="DI3">
+        <v>2.08</v>
+      </c>
+      <c r="DJ3">
+        <v>2.08</v>
+      </c>
+      <c r="DK3">
+        <v>2.08</v>
+      </c>
+      <c r="DL3">
+        <v>2.08</v>
+      </c>
+      <c r="DM3">
+        <v>2.08</v>
+      </c>
+      <c r="DN3">
+        <v>2.08</v>
+      </c>
+      <c r="DO3">
+        <v>2.08</v>
+      </c>
+      <c r="DP3">
+        <v>2.08</v>
+      </c>
+      <c r="DQ3">
+        <v>2.08</v>
+      </c>
+      <c r="DR3">
+        <v>2.08</v>
+      </c>
+      <c r="DS3">
+        <v>2.08</v>
+      </c>
+      <c r="DT3">
+        <v>2.010000000000001</v>
+      </c>
+      <c r="DU3">
+        <v>2.010000000000001</v>
+      </c>
+      <c r="DV3">
+        <v>2.010000000000001</v>
+      </c>
+      <c r="DW3">
+        <v>2.010000000000001</v>
+      </c>
+      <c r="DX3">
+        <v>2.010000000000001</v>
+      </c>
+      <c r="DY3">
+        <v>2.000000000000001</v>
+      </c>
+      <c r="DZ3">
+        <v>2.000000000000001</v>
+      </c>
+      <c r="EA3">
+        <v>2.000000000000001</v>
+      </c>
+      <c r="EB3">
+        <v>2.000000000000001</v>
+      </c>
+      <c r="EC3">
+        <v>0.6600000000000004</v>
+      </c>
+      <c r="ED3">
+        <v>0.6600000000000004</v>
+      </c>
+      <c r="EE3">
+        <v>0.6600000000000004</v>
+      </c>
+      <c r="EF3">
+        <v>0.6600000000000004</v>
+      </c>
+      <c r="EG3">
+        <v>0.6600000000000004</v>
+      </c>
+      <c r="EH3">
+        <v>0.6600000000000004</v>
+      </c>
+      <c r="EI3">
+        <v>0.6600000000000004</v>
+      </c>
+      <c r="EJ3">
+        <v>0.6600000000000004</v>
+      </c>
+      <c r="EK3">
+        <v>0.6600000000000004</v>
+      </c>
+      <c r="EL3">
+        <v>0.6600000000000004</v>
+      </c>
+      <c r="EM3">
+        <v>0.6600000000000004</v>
+      </c>
+      <c r="EN3">
+        <v>0.6600000000000004</v>
+      </c>
+      <c r="EO3">
+        <v>0.6600000000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:145">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -35718,13 +37380,430 @@
         <v>6.718412510414964</v>
       </c>
       <c r="D4">
-        <v>6.718412510414964</v>
+        <v>6.7089736737571</v>
       </c>
       <c r="E4">
-        <v>6.7089736737571</v>
+        <v>3.941502508049325</v>
       </c>
       <c r="F4">
-        <v>6.7089736737571</v>
+        <v>3.941502508048643</v>
+      </c>
+      <c r="G4">
+        <v>3.941502508048643</v>
+      </c>
+      <c r="H4">
+        <v>3.941502508048643</v>
+      </c>
+      <c r="I4">
+        <v>3.941502508048643</v>
+      </c>
+      <c r="J4">
+        <v>3.941502508048416</v>
+      </c>
+      <c r="K4">
+        <v>3.933209944208556</v>
+      </c>
+      <c r="L4">
+        <v>3.933209944208329</v>
+      </c>
+      <c r="M4">
+        <v>8.620160216306203</v>
+      </c>
+      <c r="N4">
+        <v>8.620160216306203</v>
+      </c>
+      <c r="O4">
+        <v>8.620160216306203</v>
+      </c>
+      <c r="P4">
+        <v>8.620160216306203</v>
+      </c>
+      <c r="Q4">
+        <v>8.689705333281609</v>
+      </c>
+      <c r="R4">
+        <v>1.960438712822906</v>
+      </c>
+      <c r="S4">
+        <v>1.960438712822906</v>
+      </c>
+      <c r="T4">
+        <v>1.960438712822906</v>
+      </c>
+      <c r="U4">
+        <v>1.960438712822906</v>
+      </c>
+      <c r="V4">
+        <v>1.960438712822906</v>
+      </c>
+      <c r="W4">
+        <v>1.960438712822906</v>
+      </c>
+      <c r="X4">
+        <v>1.960438712822906</v>
+      </c>
+      <c r="Y4">
+        <v>1.960438712822452</v>
+      </c>
+      <c r="Z4">
+        <v>1.960438712822452</v>
+      </c>
+      <c r="AA4">
+        <v>1.960438712822452</v>
+      </c>
+      <c r="AB4">
+        <v>1.960438712822452</v>
+      </c>
+      <c r="AC4">
+        <v>1.960438712821997</v>
+      </c>
+      <c r="AD4">
+        <v>1.960438712821997</v>
+      </c>
+      <c r="AE4">
+        <v>1.960438712821997</v>
+      </c>
+      <c r="AF4">
+        <v>1.960438712821997</v>
+      </c>
+      <c r="AG4">
+        <v>1.960438712821997</v>
+      </c>
+      <c r="AH4">
+        <v>1.960438712821997</v>
+      </c>
+      <c r="AI4">
+        <v>1.960438712821997</v>
+      </c>
+      <c r="AJ4">
+        <v>1.960438712821997</v>
+      </c>
+      <c r="AK4">
+        <v>1.960438712821997</v>
+      </c>
+      <c r="AL4">
+        <v>1.960438712821997</v>
+      </c>
+      <c r="AM4">
+        <v>1.960438712821997</v>
+      </c>
+      <c r="AN4">
+        <v>1.960438712821997</v>
+      </c>
+      <c r="AO4">
+        <v>1.960438712821997</v>
+      </c>
+      <c r="AP4">
+        <v>1.960438712821997</v>
+      </c>
+      <c r="AQ4">
+        <v>1.960438712821997</v>
+      </c>
+      <c r="AR4">
+        <v>1.960438712821997</v>
+      </c>
+      <c r="AS4">
+        <v>1.960438712821997</v>
+      </c>
+      <c r="AT4">
+        <v>1.960438712821997</v>
+      </c>
+      <c r="AU4">
+        <v>1.960438712821997</v>
+      </c>
+      <c r="AV4">
+        <v>1.960438712821997</v>
+      </c>
+      <c r="AW4">
+        <v>1.960438712821997</v>
+      </c>
+      <c r="AX4">
+        <v>1.960438712821997</v>
+      </c>
+      <c r="AY4">
+        <v>1.960438712821997</v>
+      </c>
+      <c r="AZ4">
+        <v>1.958965761378749</v>
+      </c>
+      <c r="BA4">
+        <v>1.958965761378749</v>
+      </c>
+      <c r="BB4">
+        <v>1.958965761378749</v>
+      </c>
+      <c r="BC4">
+        <v>1.958965761378295</v>
+      </c>
+      <c r="BD4">
+        <v>1.95896576137784</v>
+      </c>
+      <c r="BE4">
+        <v>1.95896576137784</v>
+      </c>
+      <c r="BF4">
+        <v>1.95896576137784</v>
+      </c>
+      <c r="BG4">
+        <v>3.917879418341272</v>
+      </c>
+      <c r="BH4">
+        <v>3.917879418341272</v>
+      </c>
+      <c r="BI4">
+        <v>3.917879418340817</v>
+      </c>
+      <c r="BJ4">
+        <v>3.917879418340817</v>
+      </c>
+      <c r="BK4">
+        <v>3.917879418340817</v>
+      </c>
+      <c r="BL4">
+        <v>6.768584142669852</v>
+      </c>
+      <c r="BM4">
+        <v>6.768584142669852</v>
+      </c>
+      <c r="BN4">
+        <v>6.768584142669852</v>
+      </c>
+      <c r="BO4">
+        <v>6.740517037362451</v>
+      </c>
+      <c r="BP4">
+        <v>6.740517037362451</v>
+      </c>
+      <c r="BQ4">
+        <v>6.740517037362451</v>
+      </c>
+      <c r="BR4">
+        <v>6.740517037361997</v>
+      </c>
+      <c r="BS4">
+        <v>6.740514209037656</v>
+      </c>
+      <c r="BT4">
+        <v>6.740514209037656</v>
+      </c>
+      <c r="BU4">
+        <v>6.68970462539346</v>
+      </c>
+      <c r="BV4">
+        <v>6.68970462539346</v>
+      </c>
+      <c r="BW4">
+        <v>6.68970462539346</v>
+      </c>
+      <c r="BX4">
+        <v>6.689701697053124</v>
+      </c>
+      <c r="BY4">
+        <v>6.689701697053124</v>
+      </c>
+      <c r="BZ4">
+        <v>6.689701697053124</v>
+      </c>
+      <c r="CA4">
+        <v>6.689701697053124</v>
+      </c>
+      <c r="CB4">
+        <v>6.689701697053124</v>
+      </c>
+      <c r="CC4">
+        <v>6.689701697053124</v>
+      </c>
+      <c r="CD4">
+        <v>6.689701697052897</v>
+      </c>
+      <c r="CE4">
+        <v>6.689701697052897</v>
+      </c>
+      <c r="CF4">
+        <v>6.689701697052897</v>
+      </c>
+      <c r="CG4">
+        <v>1.975086749121601</v>
+      </c>
+      <c r="CH4">
+        <v>1.975086749121601</v>
+      </c>
+      <c r="CI4">
+        <v>1.975086749121601</v>
+      </c>
+      <c r="CJ4">
+        <v>1.975086749121601</v>
+      </c>
+      <c r="CK4">
+        <v>1.975086749121601</v>
+      </c>
+      <c r="CL4">
+        <v>1.975086749121601</v>
+      </c>
+      <c r="CM4">
+        <v>1.975086749121601</v>
+      </c>
+      <c r="CN4">
+        <v>1.975086749121601</v>
+      </c>
+      <c r="CO4">
+        <v>1.975086749121147</v>
+      </c>
+      <c r="CP4">
+        <v>1.975086749121147</v>
+      </c>
+      <c r="CQ4">
+        <v>1.975086749121147</v>
+      </c>
+      <c r="CR4">
+        <v>1.975086749121147</v>
+      </c>
+      <c r="CS4">
+        <v>1.975086749121147</v>
+      </c>
+      <c r="CT4">
+        <v>1.975086749121147</v>
+      </c>
+      <c r="CU4">
+        <v>1.975086749121147</v>
+      </c>
+      <c r="CV4">
+        <v>1.975086749121147</v>
+      </c>
+      <c r="CW4">
+        <v>1.975086749121147</v>
+      </c>
+      <c r="CX4">
+        <v>1.975086749121147</v>
+      </c>
+      <c r="CY4">
+        <v>1.975086749121147</v>
+      </c>
+      <c r="CZ4">
+        <v>1.975086749121147</v>
+      </c>
+      <c r="DA4">
+        <v>1.975086749121147</v>
+      </c>
+      <c r="DB4">
+        <v>1.975086749121147</v>
+      </c>
+      <c r="DC4">
+        <v>1.975086749121147</v>
+      </c>
+      <c r="DD4">
+        <v>1.975086749120692</v>
+      </c>
+      <c r="DE4">
+        <v>1.975086749120692</v>
+      </c>
+      <c r="DF4">
+        <v>1.975086749120692</v>
+      </c>
+      <c r="DG4">
+        <v>1.975086749120692</v>
+      </c>
+      <c r="DH4">
+        <v>1.973195708863386</v>
+      </c>
+      <c r="DI4">
+        <v>1.973195708863386</v>
+      </c>
+      <c r="DJ4">
+        <v>1.973195708863386</v>
+      </c>
+      <c r="DK4">
+        <v>1.973195708863386</v>
+      </c>
+      <c r="DL4">
+        <v>1.973195708863386</v>
+      </c>
+      <c r="DM4">
+        <v>1.973195708863386</v>
+      </c>
+      <c r="DN4">
+        <v>1.973195708863386</v>
+      </c>
+      <c r="DO4">
+        <v>1.973195708863386</v>
+      </c>
+      <c r="DP4">
+        <v>1.973195708863386</v>
+      </c>
+      <c r="DQ4">
+        <v>1.973195708862931</v>
+      </c>
+      <c r="DR4">
+        <v>1.973195708862931</v>
+      </c>
+      <c r="DS4">
+        <v>1.973195708862477</v>
+      </c>
+      <c r="DT4">
+        <v>1.944212153974377</v>
+      </c>
+      <c r="DU4">
+        <v>1.944212153974377</v>
+      </c>
+      <c r="DV4">
+        <v>1.944212153974377</v>
+      </c>
+      <c r="DW4">
+        <v>1.944212153974377</v>
+      </c>
+      <c r="DX4">
+        <v>1.944212153973695</v>
+      </c>
+      <c r="DY4">
+        <v>1.952089136819041</v>
+      </c>
+      <c r="DZ4">
+        <v>1.952089136819041</v>
+      </c>
+      <c r="EA4">
+        <v>1.952089136818586</v>
+      </c>
+      <c r="EB4">
+        <v>1.952089136818586</v>
+      </c>
+      <c r="EC4">
+        <v>3.842115817237755</v>
+      </c>
+      <c r="ED4">
+        <v>3.842115817237755</v>
+      </c>
+      <c r="EE4">
+        <v>3.842115817237755</v>
+      </c>
+      <c r="EF4">
+        <v>3.842115817237755</v>
+      </c>
+      <c r="EG4">
+        <v>3.842115817237755</v>
+      </c>
+      <c r="EH4">
+        <v>3.842115817237755</v>
+      </c>
+      <c r="EI4">
+        <v>3.842115817237755</v>
+      </c>
+      <c r="EJ4">
+        <v>3.842043057530418</v>
+      </c>
+      <c r="EK4">
+        <v>3.830677147427423</v>
+      </c>
+      <c r="EL4">
+        <v>3.830677147427423</v>
+      </c>
+      <c r="EM4">
+        <v>3.830677147427423</v>
+      </c>
+      <c r="EN4">
+        <v>3.830677147427423</v>
+      </c>
+      <c r="EO4">
+        <v>3.830604387793073</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Increase number of generated configurations to 1000
</commit_message>
<xml_diff>
--- a/interconnection_testing.xlsx
+++ b/interconnection_testing.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="223">
   <si>
     <t>-00011110+</t>
   </si>
@@ -49,19 +49,34 @@
     <t>I_MP</t>
   </si>
   <si>
+    <t>-0110+-0011+</t>
+  </si>
+  <si>
+    <t>-1001+-1100+</t>
+  </si>
+  <si>
+    <t>-0110+-1100+</t>
+  </si>
+  <si>
     <t>-1001+-0011+</t>
   </si>
   <si>
-    <t>-0110+-0011+</t>
+    <t>-1100+-0110+</t>
   </si>
   <si>
     <t>-0011+-1001+</t>
   </si>
   <si>
-    <t>-+-(0110)0011+</t>
+    <t>-+-(1001)1100+</t>
+  </si>
+  <si>
+    <t>-+-(0110)1100+</t>
   </si>
   <si>
     <t>-00(1001)11+</t>
+  </si>
+  <si>
+    <t>-00(0110)11+</t>
   </si>
   <si>
     <t>-11(0110)00+</t>
@@ -70,16 +85,28 @@
     <t>-11(1001)00+</t>
   </si>
   <si>
-    <t>-00(0110)11+</t>
-  </si>
-  <si>
     <t>-+-11(0110)00+</t>
   </si>
   <si>
-    <t>-0011(1001)+-+</t>
+    <t>-+-11(1001)00+</t>
+  </si>
+  <si>
+    <t>-+-00(0110)11+</t>
+  </si>
+  <si>
+    <t>-+-00(1001)11+</t>
+  </si>
+  <si>
+    <t>-1100(1001)+-+</t>
+  </si>
+  <si>
+    <t>-00(0110)11+-+</t>
   </si>
   <si>
     <t>-11(0110)00+-+</t>
+  </si>
+  <si>
+    <t>-11(1001)+-00+</t>
   </si>
   <si>
     <t>-11(0110)+-00+</t>
@@ -91,259 +118,343 @@
     <t>-00(0110)+-11+</t>
   </si>
   <si>
-    <t>-11(1001)+-00+</t>
+    <t>-00+-(0110)11+</t>
   </si>
   <si>
-    <t>-11+-(1001)00+</t>
+    <t>-10010011+</t>
+  </si>
+  <si>
+    <t>-+-11000110+</t>
+  </si>
+  <si>
+    <t>-+-10011100+</t>
+  </si>
+  <si>
+    <t>-+-00111001+</t>
+  </si>
+  <si>
+    <t>-01100011+</t>
   </si>
   <si>
     <t>-+-10010011+</t>
   </si>
   <si>
-    <t>-+-11000110+</t>
-  </si>
-  <si>
-    <t>-10010011+</t>
-  </si>
-  <si>
     <t>-10011100+</t>
   </si>
   <si>
-    <t>-+-10011100+</t>
+    <t>-+-01101100+</t>
   </si>
   <si>
     <t>-01101100+</t>
   </si>
   <si>
-    <t>-01100011+</t>
+    <t>-+-11001001+</t>
+  </si>
+  <si>
+    <t>-11001001+</t>
+  </si>
+  <si>
+    <t>-11000110+</t>
+  </si>
+  <si>
+    <t>-00110110+</t>
   </si>
   <si>
     <t>-00111001+</t>
   </si>
   <si>
-    <t>-11000110+</t>
+    <t>-11010010+</t>
   </si>
   <si>
-    <t>-11001001+</t>
-  </si>
-  <si>
-    <t>-00110110+</t>
+    <t>-11100001+</t>
   </si>
   <si>
     <t>-00011011+</t>
   </si>
   <si>
+    <t>-+-01111000+</t>
+  </si>
+  <si>
+    <t>-11011000+</t>
+  </si>
+  <si>
+    <t>-+-00101101+</t>
+  </si>
+  <si>
+    <t>-+-00011110+</t>
+  </si>
+  <si>
+    <t>-10110100+</t>
+  </si>
+  <si>
+    <t>-00100111+</t>
+  </si>
+  <si>
+    <t>-00101101+</t>
+  </si>
+  <si>
+    <t>-01111000+</t>
+  </si>
+  <si>
+    <t>-+-11011000+</t>
+  </si>
+  <si>
+    <t>-11100100+</t>
+  </si>
+  <si>
+    <t>-10001101+</t>
+  </si>
+  <si>
+    <t>-+-11010010+</t>
+  </si>
+  <si>
+    <t>-+-00011011+</t>
+  </si>
+  <si>
     <t>-10000111+</t>
+  </si>
+  <si>
+    <t>-+-01001110+</t>
+  </si>
+  <si>
+    <t>-+-01001011+</t>
+  </si>
+  <si>
+    <t>-01001110+</t>
+  </si>
+  <si>
+    <t>-01001011+</t>
+  </si>
+  <si>
+    <t>-01110010+</t>
+  </si>
+  <si>
+    <t>-+-00100111+</t>
+  </si>
+  <si>
+    <t>-+-10001101+</t>
+  </si>
+  <si>
+    <t>-+-11100001+</t>
   </si>
   <si>
     <t>-10110001+</t>
   </si>
   <si>
-    <t>-00100111+</t>
-  </si>
-  <si>
-    <t>-01110010+</t>
-  </si>
-  <si>
-    <t>-+-11010010+</t>
-  </si>
-  <si>
-    <t>-+-11100100+</t>
-  </si>
-  <si>
-    <t>-+-11100001+</t>
-  </si>
-  <si>
-    <t>-10110100+</t>
-  </si>
-  <si>
-    <t>-+-01001110+</t>
-  </si>
-  <si>
-    <t>-00101101+</t>
-  </si>
-  <si>
-    <t>-+-01110010+</t>
-  </si>
-  <si>
-    <t>-11100001+</t>
-  </si>
-  <si>
-    <t>-11010010+</t>
-  </si>
-  <si>
-    <t>-01111000+</t>
-  </si>
-  <si>
-    <t>-10001101+</t>
-  </si>
-  <si>
-    <t>-+-00011011+</t>
-  </si>
-  <si>
-    <t>-+-10001101+</t>
-  </si>
-  <si>
-    <t>-11100100+</t>
-  </si>
-  <si>
-    <t>-11011000+</t>
-  </si>
-  <si>
-    <t>-01001011+</t>
-  </si>
-  <si>
-    <t>-01001110+</t>
+    <t>-10010011+-+</t>
   </si>
   <si>
     <t>-10011100+-+</t>
   </si>
   <si>
+    <t>-01100011+-+</t>
+  </si>
+  <si>
     <t>-01101100+-+</t>
   </si>
   <si>
-    <t>-01100011+-+</t>
+    <t>-11001001+-+</t>
   </si>
   <si>
-    <t>-11100100+-+</t>
+    <t>-00110110+-+</t>
   </si>
   <si>
-    <t>-00101101+-+</t>
+    <t>-11011000+-+</t>
+  </si>
+  <si>
+    <t>-00100111+-+</t>
+  </si>
+  <si>
+    <t>-00011011+-+</t>
+  </si>
+  <si>
+    <t>-00011110+-+</t>
+  </si>
+  <si>
+    <t>-10000111+-+</t>
+  </si>
+  <si>
+    <t>-01110010+-+</t>
+  </si>
+  <si>
+    <t>-01001110+-+</t>
+  </si>
+  <si>
+    <t>-11100001+-+</t>
+  </si>
+  <si>
+    <t>-10110100+-+</t>
+  </si>
+  <si>
+    <t>-10110001+-+</t>
+  </si>
+  <si>
+    <t>-01111000+-+</t>
   </si>
   <si>
     <t>-11010010+-+</t>
   </si>
   <si>
-    <t>-11100001+-+</t>
+    <t>-1011+-0100+</t>
   </si>
   <si>
-    <t>-0111+-0010+</t>
+    <t>-1000+-0111+</t>
   </si>
   <si>
-    <t>-0100+-1110+</t>
+    <t>-1000+-1101+</t>
   </si>
   <si>
-    <t>-1110+-0100+</t>
+    <t>-0111+-1000+</t>
+  </si>
+  <si>
+    <t>-0010+-0111+</t>
+  </si>
+  <si>
+    <t>-1101+-0010+</t>
   </si>
   <si>
     <t>-0010+-1101+</t>
   </si>
   <si>
-    <t>-1101+-0010+</t>
+    <t>-1101+-1000+</t>
   </si>
   <si>
-    <t>-00(1101)+-10+</t>
+    <t>-1110+-0001+</t>
   </si>
   <si>
-    <t>-11(0001)+-10+</t>
+    <t>-11(0010)+-01+</t>
+  </si>
+  <si>
+    <t>-11(0100)+-10+</t>
+  </si>
+  <si>
+    <t>-11(1000)+-01+</t>
   </si>
   <si>
     <t>-00(1011)+-01+</t>
   </si>
   <si>
-    <t>-10(1101)+-00+</t>
+    <t>-01+-(0010)11+</t>
   </si>
   <si>
-    <t>-10(0001)+-11+</t>
+    <t>-10+-(0111)00+</t>
+  </si>
+  <si>
+    <t>-01+-(1110)00+</t>
+  </si>
+  <si>
+    <t>-10+-(0100)11+</t>
   </si>
   <si>
     <t>-01(0010)+-11+</t>
   </si>
   <si>
+    <t>-01(1110)+-00+</t>
+  </si>
+  <si>
+    <t>-10(1101)+-00+</t>
+  </si>
+  <si>
+    <t>-10(0111)+-00+</t>
+  </si>
+  <si>
     <t>-01(1011)+-00+</t>
+  </si>
+  <si>
+    <t>-110110+-00+</t>
+  </si>
+  <si>
+    <t>-011011+-00+</t>
+  </si>
+  <si>
+    <t>-011000+-11+</t>
   </si>
   <si>
     <t>-100100+-11+</t>
   </si>
   <si>
-    <t>-011000+-11+</t>
+    <t>-010010+-11+</t>
   </si>
   <si>
-    <t>-11+-(0100)10+</t>
+    <t>-100111+-00+</t>
+  </si>
+  <si>
+    <t>-001001+-11+</t>
+  </si>
+  <si>
+    <t>-011110+-00+</t>
+  </si>
+  <si>
+    <t>-111001+-00+</t>
+  </si>
+  <si>
+    <t>-000110+-11+</t>
+  </si>
+  <si>
+    <t>-11+-(0001)10+</t>
   </si>
   <si>
     <t>-00+-(1110)01+</t>
   </si>
   <si>
+    <t>-00+-(1101)10+</t>
+  </si>
+  <si>
     <t>-11+-(1000)01+</t>
+  </si>
+  <si>
+    <t>-00+-(1011)01+</t>
+  </si>
+  <si>
+    <t>-00+-111001+</t>
+  </si>
+  <si>
+    <t>-00+-011011+</t>
   </si>
   <si>
     <t>-11+-011000+</t>
   </si>
   <si>
-    <t>-11+-000110+</t>
+    <t>-11+-100100+</t>
   </si>
   <si>
-    <t>-00+-111001+</t>
-  </si>
-  <si>
-    <t>-11+-100100+</t>
+    <t>-11+-001001+</t>
   </si>
   <si>
     <t>-00+-100111+</t>
   </si>
   <si>
-    <t>-00+-110110+</t>
-  </si>
-  <si>
     <t>-00+-011110+</t>
   </si>
   <si>
-    <t>-11+-100001+</t>
+    <t>-00+-101101+</t>
   </si>
   <si>
     <t>-11+-010010+</t>
   </si>
   <si>
-    <t>-10(1101)00+</t>
-  </si>
-  <si>
-    <t>-01(0010)11+</t>
+    <t>-01(1011)00+</t>
   </si>
   <si>
     <t>-10(0100)11+</t>
   </si>
   <si>
-    <t>-10(0001)11+</t>
+    <t>-01(1110)00+</t>
   </si>
   <si>
-    <t>-01(1011)00+</t>
+    <t>-10(1101)00+</t>
+  </si>
+  <si>
+    <t>-10(0111)00+</t>
   </si>
   <si>
     <t>-01(1000)11+</t>
   </si>
   <si>
-    <t>-01(1110)00+</t>
+    <t>-10(0001)11+</t>
   </si>
   <si>
-    <t>-10(0111)00+</t>
-  </si>
-  <si>
-    <t>-00(1110)01+</t>
-  </si>
-  <si>
-    <t>-+-(1110)0001+</t>
-  </si>
-  <si>
-    <t>-+-01(1110)00+</t>
-  </si>
-  <si>
-    <t>-11(0001)10+</t>
-  </si>
-  <si>
-    <t>-+-01(1011)00+</t>
-  </si>
-  <si>
-    <t>-+-(0100)1011+</t>
-  </si>
-  <si>
-    <t>-11(0010)01+</t>
-  </si>
-  <si>
-    <t>-+-11(0001)10+</t>
-  </si>
-  <si>
-    <t>-+-(0010)0111+</t>
+    <t>-01(0010)11+</t>
   </si>
   <si>
     <t>-+-(0111)1000+</t>
@@ -352,127 +463,229 @@
     <t>-+-(1011)0001+</t>
   </si>
   <si>
+    <t>-+-01(1011)00+</t>
+  </si>
+  <si>
+    <t>-00(1110)01+</t>
+  </si>
+  <si>
+    <t>-+-(1110)0100+</t>
+  </si>
+  <si>
+    <t>-+-(1000)1101+</t>
+  </si>
+  <si>
+    <t>-+-(0010)1101+</t>
+  </si>
+  <si>
+    <t>-+-11(0100)10+</t>
+  </si>
+  <si>
+    <t>-+-(0001)1110+</t>
+  </si>
+  <si>
+    <t>-11(0010)01+</t>
+  </si>
+  <si>
+    <t>-+-(0010)0111+</t>
+  </si>
+  <si>
     <t>-+-10(0001)11+</t>
+  </si>
+  <si>
+    <t>-+-00(1110)01+</t>
+  </si>
+  <si>
+    <t>-11(0001)10+</t>
+  </si>
+  <si>
+    <t>-+-00(1011)01+</t>
+  </si>
+  <si>
+    <t>-+-(0001)1011+</t>
+  </si>
+  <si>
+    <t>-+-(0100)1011+</t>
+  </si>
+  <si>
+    <t>-+-01(0010)11+</t>
+  </si>
+  <si>
+    <t>-+-(0111)0010+</t>
   </si>
   <si>
     <t>-00(1101)10+</t>
   </si>
   <si>
-    <t>-+-(1101)1000+</t>
+    <t>-+-11(0001)10+</t>
   </si>
   <si>
-    <t>-+-(0001)1110+</t>
+    <t>-+-(1110)0001+</t>
+  </si>
+  <si>
+    <t>-+-00(1101)10+</t>
+  </si>
+  <si>
+    <t>-11(1000)01+</t>
+  </si>
+  <si>
+    <t>-00(1011)01+</t>
   </si>
   <si>
     <t>-11(0100)10+</t>
   </si>
   <si>
-    <t>-00(1011)01+</t>
+    <t>-0010(1101)+-+</t>
   </si>
   <si>
-    <t>-11(1000)01+</t>
+    <t>-11(1000)01+-+</t>
   </si>
   <si>
-    <t>-0100(1011)+-+</t>
+    <t>-1101(0010)+-+</t>
+  </si>
+  <si>
+    <t>-11(0100)10+-+</t>
+  </si>
+  <si>
+    <t>-00(1110)01+-+</t>
+  </si>
+  <si>
+    <t>-00(0111)10+-+</t>
+  </si>
+  <si>
+    <t>-10(0111)00+-+</t>
+  </si>
+  <si>
+    <t>-11(0010)01+-+</t>
   </si>
   <si>
     <t>-01(1011)00+-+</t>
   </si>
   <si>
-    <t>-10(0100)11+-+</t>
+    <t>-0111(1000)+-+</t>
   </si>
   <si>
     <t>-11(0001)10+-+</t>
   </si>
   <si>
-    <t>-1011(0001)+-+</t>
+    <t>-00(1101)10+-+</t>
   </si>
   <si>
-    <t>-11(0100)10+-+</t>
+    <t>-00(1011)01+-+</t>
   </si>
   <si>
-    <t>-1000(1101)+-+</t>
+    <t>-0111(0010)+-+</t>
   </si>
   <si>
-    <t>-1000(0111)+-+</t>
+    <t>-10(0001)11+-+</t>
   </si>
   <si>
-    <t>-00(1110)01+-+</t>
+    <t>-1101(1000)+-+</t>
   </si>
   <si>
-    <t>-10(1101)00+-+</t>
-  </si>
-  <si>
-    <t>-01(1110)00+-+</t>
+    <t>-1110(0100)+-+</t>
   </si>
   <si>
     <t>-0010(0111)+-+</t>
   </si>
   <si>
+    <t>-10(1100)01+</t>
+  </si>
+  <si>
     <t>-10(0011)01+</t>
   </si>
   <si>
-    <t>-10(1100)01+</t>
+    <t>-01(0011)10+</t>
   </si>
   <si>
     <t>-01(1100)10+</t>
   </si>
   <si>
-    <t>-01(0011)10+</t>
+    <t>-+-10(0011)01+</t>
+  </si>
+  <si>
+    <t>-+-(0011)1001+</t>
+  </si>
+  <si>
+    <t>-+-(1100)0110+</t>
   </si>
   <si>
     <t>-+-01(1100)10+</t>
   </si>
   <si>
-    <t>-1001(0011)+-+</t>
-  </si>
-  <si>
-    <t>-1001(1100)+-+</t>
-  </si>
-  <si>
-    <t>-10(0011)01+-+</t>
+    <t>-0110(1100)+-+</t>
   </si>
   <si>
     <t>-01(0011)10+-+</t>
   </si>
   <si>
+    <t>-011100+-10+</t>
+  </si>
+  <si>
     <t>-010011+-10+</t>
+  </si>
+  <si>
+    <t>-000111+-10+</t>
+  </si>
+  <si>
+    <t>-001011+-01+</t>
+  </si>
+  <si>
+    <t>-001110+-01+</t>
   </si>
   <si>
     <t>-001101+-10+</t>
   </si>
   <si>
-    <t>-001011+-01+</t>
+    <t>-110010+-01+</t>
   </si>
   <si>
-    <t>-000111+-10+</t>
+    <t>-101100+-01+</t>
   </si>
   <si>
-    <t>-110001+-10+</t>
+    <t>-110100+-10+</t>
   </si>
   <si>
     <t>-111000+-01+</t>
   </si>
   <si>
-    <t>-110010+-01+</t>
+    <t>-01(1100)+-10+</t>
   </si>
   <si>
-    <t>-01(0011)+-10+</t>
+    <t>-10(0011)+-01+</t>
+  </si>
+  <si>
+    <t>-10(1100)+-01+</t>
+  </si>
+  <si>
+    <t>-01+-001110+</t>
+  </si>
+  <si>
+    <t>-01+-110010+</t>
   </si>
   <si>
     <t>-01+-001011+</t>
   </si>
   <si>
-    <t>-01+-110010+</t>
+    <t>-10+-000111+</t>
+  </si>
+  <si>
+    <t>-10+-110100+</t>
   </si>
   <si>
     <t>-10+-110001+</t>
   </si>
   <si>
-    <t>-10+-000111+</t>
+    <t>-10+-010011+</t>
   </si>
   <si>
-    <t>-01+-(0011)10+</t>
+    <t>-10+-001101+</t>
+  </si>
+  <si>
+    <t>-01+-(1100)10+</t>
+  </si>
+  <si>
+    <t>-10+-(0011)01+</t>
   </si>
 </sst>
 </file>
@@ -36055,13 +36268,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:EO4"/>
+  <dimension ref="A1:HI4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:145">
+    <row r="1" spans="1:217">
       <c r="B1" s="1" t="s">
         <v>10</v>
       </c>
@@ -36177,34 +36390,34 @@
         <v>47</v>
       </c>
       <c r="AN1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AW1" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AT1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="AV1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AW1" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="AX1" s="1" t="s">
         <v>57</v>
@@ -36336,61 +36549,61 @@
         <v>99</v>
       </c>
       <c r="CO1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="CP1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="CP1" s="1" t="s">
+      <c r="CQ1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="CQ1" s="1" t="s">
+      <c r="CR1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="CR1" s="1" t="s">
+      <c r="CS1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="CS1" s="1" t="s">
+      <c r="CT1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="CT1" s="1" t="s">
+      <c r="CU1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="CU1" s="1" t="s">
+      <c r="CV1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="CV1" s="1" t="s">
+      <c r="CW1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="CW1" s="1" t="s">
+      <c r="CX1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="CX1" s="1" t="s">
+      <c r="CY1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="CY1" s="1" t="s">
+      <c r="CZ1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="CZ1" s="1" t="s">
+      <c r="DA1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="DA1" s="1" t="s">
+      <c r="DB1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="DB1" s="1" t="s">
+      <c r="DC1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="DC1" s="1" t="s">
+      <c r="DD1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="DD1" s="1" t="s">
+      <c r="DE1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="DE1" s="1" t="s">
+      <c r="DF1" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="DF1" s="1" t="s">
+      <c r="DG1" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="DG1" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="DH1" s="1" t="s">
         <v>118</v>
@@ -36494,8 +36707,224 @@
       <c r="EO1" s="1" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="2" spans="1:145">
+      <c r="EP1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="EQ1" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="ER1" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="ES1" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="ET1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="EU1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="EV1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="EW1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="EX1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="EY1" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="EZ1" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="FA1" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="FB1" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="FC1" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="FD1" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="FE1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="FF1" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="FG1" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="FH1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="FI1" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="FJ1" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="FK1" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="FL1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="FM1" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="FN1" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="FO1" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="FP1" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="FQ1" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="FR1" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="FS1" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="FT1" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="FU1" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="FV1" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="FW1" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="FX1" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="FY1" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="FZ1" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="GA1" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="GB1" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="GC1" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="GD1" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="GE1" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="GF1" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="GG1" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="GH1" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="GI1" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="GJ1" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="GK1" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="GL1" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="GM1" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="GN1" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="GO1" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="GP1" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="GQ1" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="GR1" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="GS1" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="GT1" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="GU1" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="GV1" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="GW1" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="GX1" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="GY1" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="GZ1" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="HA1" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="HB1" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="HC1" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="HD1" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="HE1" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="HF1" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="HG1" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="HH1" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="HI1" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="2" spans="1:217">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -36506,112 +36935,112 @@
         <v>8.801120388643609</v>
       </c>
       <c r="D2">
+        <v>8.801120388643609</v>
+      </c>
+      <c r="E2">
+        <v>8.801120388643609</v>
+      </c>
+      <c r="F2">
         <v>8.788755512621808</v>
       </c>
-      <c r="E2">
+      <c r="G2">
+        <v>8.788755512621808</v>
+      </c>
+      <c r="H2">
         <v>8.001250091340133</v>
       </c>
-      <c r="F2">
+      <c r="I2">
+        <v>8.001250091340133</v>
+      </c>
+      <c r="J2">
         <v>8.001250091338749</v>
       </c>
-      <c r="G2">
+      <c r="K2">
         <v>8.001250091338749</v>
       </c>
-      <c r="H2">
+      <c r="L2">
         <v>8.001250091338749</v>
       </c>
-      <c r="I2">
+      <c r="M2">
         <v>8.001250091338749</v>
       </c>
-      <c r="J2">
+      <c r="N2">
         <v>8.001250091338287</v>
       </c>
-      <c r="K2">
+      <c r="O2">
+        <v>8.001250091338287</v>
+      </c>
+      <c r="P2">
+        <v>8.001250091338287</v>
+      </c>
+      <c r="Q2">
+        <v>8.001250091338287</v>
+      </c>
+      <c r="R2">
         <v>7.984416186743372</v>
       </c>
-      <c r="L2">
+      <c r="S2">
         <v>7.98441618674291</v>
       </c>
-      <c r="M2">
+      <c r="T2">
+        <v>7.98441618674291</v>
+      </c>
+      <c r="U2">
         <v>5.861708947088221</v>
       </c>
-      <c r="N2">
+      <c r="V2">
         <v>5.861708947088221</v>
       </c>
-      <c r="O2">
+      <c r="W2">
         <v>5.861708947088221</v>
       </c>
-      <c r="P2">
+      <c r="X2">
         <v>5.861708947088221</v>
       </c>
-      <c r="Q2">
+      <c r="Y2">
         <v>5.822102573298681</v>
       </c>
-      <c r="R2">
+      <c r="Z2">
         <v>5.332393298878278</v>
       </c>
-      <c r="S2">
+      <c r="AA2">
         <v>5.332393298878278</v>
       </c>
-      <c r="T2">
+      <c r="AB2">
         <v>5.332393298878278</v>
       </c>
-      <c r="U2">
+      <c r="AC2">
         <v>5.332393298878278</v>
       </c>
-      <c r="V2">
+      <c r="AD2">
         <v>5.332393298878278</v>
       </c>
-      <c r="W2">
+      <c r="AE2">
         <v>5.332393298878278</v>
       </c>
-      <c r="X2">
+      <c r="AF2">
         <v>5.332393298878278</v>
       </c>
-      <c r="Y2">
+      <c r="AG2">
+        <v>5.332393298878278</v>
+      </c>
+      <c r="AH2">
+        <v>5.332393298878278</v>
+      </c>
+      <c r="AI2">
+        <v>5.332393298878278</v>
+      </c>
+      <c r="AJ2">
         <v>5.332393298877041</v>
       </c>
-      <c r="Z2">
+      <c r="AK2">
         <v>5.332393298877041</v>
       </c>
-      <c r="AA2">
+      <c r="AL2">
         <v>5.332393298877041</v>
       </c>
-      <c r="AB2">
+      <c r="AM2">
         <v>5.332393298877041</v>
-      </c>
-      <c r="AC2">
-        <v>5.332393298875804</v>
-      </c>
-      <c r="AD2">
-        <v>5.332393298875804</v>
-      </c>
-      <c r="AE2">
-        <v>5.332393298875804</v>
-      </c>
-      <c r="AF2">
-        <v>5.332393298875804</v>
-      </c>
-      <c r="AG2">
-        <v>5.332393298875804</v>
-      </c>
-      <c r="AH2">
-        <v>5.332393298875804</v>
-      </c>
-      <c r="AI2">
-        <v>5.332393298875804</v>
-      </c>
-      <c r="AJ2">
-        <v>5.332393298875804</v>
-      </c>
-      <c r="AK2">
-        <v>5.332393298875804</v>
-      </c>
-      <c r="AL2">
-        <v>5.332393298875804</v>
-      </c>
-      <c r="AM2">
-        <v>5.332393298875804</v>
       </c>
       <c r="AN2">
         <v>5.332393298875804</v>
@@ -36650,289 +37079,505 @@
         <v>5.332393298875804</v>
       </c>
       <c r="AZ2">
+        <v>5.332393298875804</v>
+      </c>
+      <c r="BA2">
+        <v>5.332393298875804</v>
+      </c>
+      <c r="BB2">
+        <v>5.332393298875804</v>
+      </c>
+      <c r="BC2">
+        <v>5.332393298875804</v>
+      </c>
+      <c r="BD2">
+        <v>5.332393298875804</v>
+      </c>
+      <c r="BE2">
+        <v>5.332393298875804</v>
+      </c>
+      <c r="BF2">
+        <v>5.332393298875804</v>
+      </c>
+      <c r="BG2">
+        <v>5.332393298875804</v>
+      </c>
+      <c r="BH2">
+        <v>5.332393298875804</v>
+      </c>
+      <c r="BI2">
+        <v>5.332393298875804</v>
+      </c>
+      <c r="BJ2">
+        <v>5.332393298875804</v>
+      </c>
+      <c r="BK2">
+        <v>5.332393298875804</v>
+      </c>
+      <c r="BL2">
+        <v>5.332393298875804</v>
+      </c>
+      <c r="BM2">
+        <v>5.332393298875804</v>
+      </c>
+      <c r="BN2">
+        <v>5.332393298875804</v>
+      </c>
+      <c r="BO2">
         <v>5.328386870950171</v>
       </c>
-      <c r="BA2">
+      <c r="BP2">
         <v>5.328386870950171</v>
       </c>
-      <c r="BB2">
+      <c r="BQ2">
         <v>5.328386870950171</v>
       </c>
-      <c r="BC2">
+      <c r="BR2">
+        <v>5.328386870950171</v>
+      </c>
+      <c r="BS2">
         <v>5.328386870948934</v>
       </c>
-      <c r="BD2">
+      <c r="BT2">
+        <v>5.328386870948934</v>
+      </c>
+      <c r="BU2">
+        <v>5.328386870948934</v>
+      </c>
+      <c r="BV2">
+        <v>5.328386870948934</v>
+      </c>
+      <c r="BW2">
+        <v>5.328386870948934</v>
+      </c>
+      <c r="BX2">
         <v>5.328386870947697</v>
       </c>
-      <c r="BE2">
+      <c r="BY2">
         <v>5.328386870947697</v>
       </c>
-      <c r="BF2">
+      <c r="BZ2">
         <v>5.328386870947697</v>
       </c>
-      <c r="BG2">
+      <c r="CA2">
+        <v>5.328386870947697</v>
+      </c>
+      <c r="CB2">
+        <v>5.328386870947697</v>
+      </c>
+      <c r="CC2">
+        <v>5.328386870947697</v>
+      </c>
+      <c r="CD2">
+        <v>5.328386870947697</v>
+      </c>
+      <c r="CE2">
+        <v>5.328386870947697</v>
+      </c>
+      <c r="CF2">
+        <v>5.328386870947697</v>
+      </c>
+      <c r="CG2">
         <v>5.328316008944133</v>
       </c>
-      <c r="BH2">
+      <c r="CH2">
         <v>5.328316008944133</v>
       </c>
-      <c r="BI2">
+      <c r="CI2">
+        <v>5.328316008944133</v>
+      </c>
+      <c r="CJ2">
+        <v>5.328316008944133</v>
+      </c>
+      <c r="CK2">
         <v>5.328316008943515</v>
       </c>
-      <c r="BJ2">
+      <c r="CL2">
         <v>5.328316008943515</v>
       </c>
-      <c r="BK2">
+      <c r="CM2">
         <v>5.328316008943515</v>
       </c>
-      <c r="BL2">
+      <c r="CN2">
+        <v>5.328316008943515</v>
+      </c>
+      <c r="CO2">
+        <v>5.328316008943515</v>
+      </c>
+      <c r="CP2">
+        <v>5.328316008943515</v>
+      </c>
+      <c r="CQ2">
         <v>4.534951375588803</v>
       </c>
-      <c r="BM2">
+      <c r="CR2">
         <v>4.534951375588803</v>
       </c>
-      <c r="BN2">
+      <c r="CS2">
         <v>4.534951375588803</v>
       </c>
-      <c r="BO2">
+      <c r="CT2">
+        <v>4.534951375588803</v>
+      </c>
+      <c r="CU2">
+        <v>4.524226195118227</v>
+      </c>
+      <c r="CV2">
+        <v>4.524226195118227</v>
+      </c>
+      <c r="CW2">
+        <v>4.524226195118227</v>
+      </c>
+      <c r="CX2">
+        <v>4.524226195118227</v>
+      </c>
+      <c r="CY2">
         <v>4.516146415032845</v>
       </c>
-      <c r="BP2">
+      <c r="CZ2">
         <v>4.516146415032845</v>
       </c>
-      <c r="BQ2">
+      <c r="DA2">
         <v>4.516146415032845</v>
       </c>
-      <c r="BR2">
+      <c r="DB2">
         <v>4.51614641503254</v>
       </c>
-      <c r="BS2">
+      <c r="DC2">
+        <v>4.51614641503254</v>
+      </c>
+      <c r="DD2">
         <v>4.516144520055231</v>
       </c>
-      <c r="BT2">
+      <c r="DE2">
         <v>4.516144520055231</v>
       </c>
-      <c r="BU2">
+      <c r="DF2">
+        <v>4.516144520055231</v>
+      </c>
+      <c r="DG2">
+        <v>4.516144520055231</v>
+      </c>
+      <c r="DH2">
+        <v>4.516144520055231</v>
+      </c>
+      <c r="DI2">
+        <v>4.516144520055231</v>
+      </c>
+      <c r="DJ2">
+        <v>4.516144520055231</v>
+      </c>
+      <c r="DK2">
+        <v>4.516144520055231</v>
+      </c>
+      <c r="DL2">
+        <v>4.516144520055231</v>
+      </c>
+      <c r="DM2">
+        <v>4.516144520055231</v>
+      </c>
+      <c r="DN2">
         <v>4.482102099013621</v>
       </c>
-      <c r="BV2">
+      <c r="DO2">
         <v>4.482102099013621</v>
       </c>
-      <c r="BW2">
+      <c r="DP2">
         <v>4.482102099013621</v>
       </c>
-      <c r="BX2">
+      <c r="DQ2">
+        <v>4.482102099013621</v>
+      </c>
+      <c r="DR2">
+        <v>4.482102099013621</v>
+      </c>
+      <c r="DS2">
         <v>4.482100137025595</v>
       </c>
-      <c r="BY2">
+      <c r="DT2">
         <v>4.482100137025595</v>
       </c>
-      <c r="BZ2">
+      <c r="DU2">
         <v>4.482100137025595</v>
       </c>
-      <c r="CA2">
+      <c r="DV2">
         <v>4.482100137025595</v>
       </c>
-      <c r="CB2">
+      <c r="DW2">
         <v>4.482100137025595</v>
       </c>
-      <c r="CC2">
+      <c r="DX2">
         <v>4.482100137025595</v>
       </c>
-      <c r="CD2">
+      <c r="DY2">
         <v>4.482100137025443</v>
       </c>
-      <c r="CE2">
+      <c r="DZ2">
         <v>4.482100137025443</v>
       </c>
-      <c r="CF2">
+      <c r="EA2">
         <v>4.482100137025443</v>
       </c>
-      <c r="CG2">
+      <c r="EB2">
         <v>4.10818043817293</v>
       </c>
-      <c r="CH2">
+      <c r="EC2">
         <v>4.10818043817293</v>
       </c>
-      <c r="CI2">
+      <c r="ED2">
         <v>4.10818043817293</v>
       </c>
-      <c r="CJ2">
+      <c r="EE2">
         <v>4.10818043817293</v>
       </c>
-      <c r="CK2">
+      <c r="EF2">
         <v>4.10818043817293</v>
       </c>
-      <c r="CL2">
+      <c r="EG2">
         <v>4.10818043817293</v>
       </c>
-      <c r="CM2">
+      <c r="EH2">
         <v>4.10818043817293</v>
       </c>
-      <c r="CN2">
+      <c r="EI2">
         <v>4.10818043817293</v>
       </c>
-      <c r="CO2">
+      <c r="EJ2">
         <v>4.108180438171984</v>
       </c>
-      <c r="CP2">
+      <c r="EK2">
         <v>4.108180438171984</v>
       </c>
-      <c r="CQ2">
+      <c r="EL2">
         <v>4.108180438171984</v>
       </c>
-      <c r="CR2">
+      <c r="EM2">
         <v>4.108180438171984</v>
       </c>
-      <c r="CS2">
+      <c r="EN2">
         <v>4.108180438171984</v>
       </c>
-      <c r="CT2">
+      <c r="EO2">
         <v>4.108180438171984</v>
       </c>
-      <c r="CU2">
+      <c r="EP2">
         <v>4.108180438171984</v>
       </c>
-      <c r="CV2">
+      <c r="EQ2">
         <v>4.108180438171984</v>
       </c>
-      <c r="CW2">
+      <c r="ER2">
         <v>4.108180438171984</v>
       </c>
-      <c r="CX2">
+      <c r="ES2">
         <v>4.108180438171984</v>
       </c>
-      <c r="CY2">
+      <c r="ET2">
         <v>4.108180438171984</v>
       </c>
-      <c r="CZ2">
+      <c r="EU2">
         <v>4.108180438171984</v>
       </c>
-      <c r="DA2">
+      <c r="EV2">
         <v>4.108180438171984</v>
       </c>
-      <c r="DB2">
+      <c r="EW2">
         <v>4.108180438171984</v>
       </c>
-      <c r="DC2">
+      <c r="EX2">
         <v>4.108180438171984</v>
       </c>
-      <c r="DD2">
+      <c r="EY2">
+        <v>4.108180438171984</v>
+      </c>
+      <c r="EZ2">
+        <v>4.108180438171984</v>
+      </c>
+      <c r="FA2">
+        <v>4.108180438171984</v>
+      </c>
+      <c r="FB2">
+        <v>4.108180438171984</v>
+      </c>
+      <c r="FC2">
+        <v>4.108180438171984</v>
+      </c>
+      <c r="FD2">
+        <v>4.108180438171984</v>
+      </c>
+      <c r="FE2">
+        <v>4.108180438171984</v>
+      </c>
+      <c r="FF2">
+        <v>4.108180438171984</v>
+      </c>
+      <c r="FG2">
         <v>4.108180438171038</v>
       </c>
-      <c r="DE2">
+      <c r="FH2">
         <v>4.108180438171038</v>
       </c>
-      <c r="DF2">
+      <c r="FI2">
         <v>4.108180438171038</v>
       </c>
-      <c r="DG2">
+      <c r="FJ2">
         <v>4.108180438171038</v>
       </c>
-      <c r="DH2">
+      <c r="FK2">
         <v>4.104247074435842</v>
       </c>
-      <c r="DI2">
+      <c r="FL2">
         <v>4.104247074435842</v>
       </c>
-      <c r="DJ2">
+      <c r="FM2">
         <v>4.104247074435842</v>
       </c>
-      <c r="DK2">
+      <c r="FN2">
         <v>4.104247074435842</v>
       </c>
-      <c r="DL2">
+      <c r="FO2">
         <v>4.104247074435842</v>
       </c>
-      <c r="DM2">
+      <c r="FP2">
         <v>4.104247074435842</v>
       </c>
-      <c r="DN2">
+      <c r="FQ2">
         <v>4.104247074435842</v>
       </c>
-      <c r="DO2">
+      <c r="FR2">
         <v>4.104247074435842</v>
       </c>
-      <c r="DP2">
+      <c r="FS2">
         <v>4.104247074435842</v>
       </c>
-      <c r="DQ2">
+      <c r="FT2">
+        <v>4.104247074435842</v>
+      </c>
+      <c r="FU2">
+        <v>4.104247074435842</v>
+      </c>
+      <c r="FV2">
+        <v>4.104247074435842</v>
+      </c>
+      <c r="FW2">
+        <v>4.104247074435842</v>
+      </c>
+      <c r="FX2">
+        <v>4.104247074435842</v>
+      </c>
+      <c r="FY2">
         <v>4.104247074434896</v>
       </c>
-      <c r="DR2">
-        <v>4.104247074434896</v>
-      </c>
-      <c r="DS2">
+      <c r="FZ2">
         <v>4.104247074433951</v>
       </c>
-      <c r="DT2">
+      <c r="GA2">
+        <v>4.104247074433951</v>
+      </c>
+      <c r="GB2">
+        <v>4.104247074433951</v>
+      </c>
+      <c r="GC2">
         <v>3.907866429488499</v>
       </c>
-      <c r="DU2">
+      <c r="GD2">
         <v>3.907866429488499</v>
       </c>
-      <c r="DV2">
+      <c r="GE2">
         <v>3.907866429488499</v>
       </c>
-      <c r="DW2">
+      <c r="GF2">
         <v>3.907866429488499</v>
       </c>
-      <c r="DX2">
+      <c r="GG2">
         <v>3.907866429487128</v>
       </c>
-      <c r="DY2">
+      <c r="GH2">
+        <v>3.907866429487128</v>
+      </c>
+      <c r="GI2">
+        <v>3.907866429487128</v>
+      </c>
+      <c r="GJ2">
+        <v>3.907866429487128</v>
+      </c>
+      <c r="GK2">
         <v>3.904178273638084</v>
       </c>
-      <c r="DZ2">
-        <v>3.904178273638084</v>
-      </c>
-      <c r="EA2">
+      <c r="GL2">
         <v>3.904178273637174</v>
       </c>
-      <c r="EB2">
-        <v>3.904178273637174</v>
-      </c>
-      <c r="EC2">
+      <c r="GM2">
         <v>2.535796439376919</v>
       </c>
-      <c r="ED2">
+      <c r="GN2">
         <v>2.535796439376919</v>
       </c>
-      <c r="EE2">
+      <c r="GO2">
         <v>2.535796439376919</v>
       </c>
-      <c r="EF2">
+      <c r="GP2">
         <v>2.535796439376919</v>
       </c>
-      <c r="EG2">
+      <c r="GQ2">
         <v>2.535796439376919</v>
       </c>
-      <c r="EH2">
+      <c r="GR2">
         <v>2.535796439376919</v>
       </c>
-      <c r="EI2">
+      <c r="GS2">
         <v>2.535796439376919</v>
       </c>
-      <c r="EJ2">
+      <c r="GT2">
+        <v>2.535796439376919</v>
+      </c>
+      <c r="GU2">
+        <v>2.535796439376919</v>
+      </c>
+      <c r="GV2">
+        <v>2.535796439376919</v>
+      </c>
+      <c r="GW2">
         <v>2.535748417970078</v>
       </c>
-      <c r="EK2">
+      <c r="GX2">
+        <v>2.535748417970078</v>
+      </c>
+      <c r="GY2">
+        <v>2.535748417970078</v>
+      </c>
+      <c r="GZ2">
         <v>2.5282469173021</v>
       </c>
-      <c r="EL2">
+      <c r="HA2">
         <v>2.5282469173021</v>
       </c>
-      <c r="EM2">
+      <c r="HB2">
         <v>2.5282469173021</v>
       </c>
-      <c r="EN2">
+      <c r="HC2">
         <v>2.5282469173021</v>
       </c>
-      <c r="EO2">
+      <c r="HD2">
+        <v>2.5282469173021</v>
+      </c>
+      <c r="HE2">
+        <v>2.5282469173021</v>
+      </c>
+      <c r="HF2">
+        <v>2.5282469173021</v>
+      </c>
+      <c r="HG2">
+        <v>2.5282469173021</v>
+      </c>
+      <c r="HH2">
         <v>2.52819889594343</v>
       </c>
-    </row>
-    <row r="3" spans="1:145">
+      <c r="HI2">
+        <v>2.52819889594343</v>
+      </c>
+    </row>
+    <row r="3" spans="1:217">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -36946,13 +37591,13 @@
         <v>1.310000000000001</v>
       </c>
       <c r="E3">
-        <v>2.030000000000001</v>
+        <v>1.310000000000001</v>
       </c>
       <c r="F3">
-        <v>2.030000000000001</v>
+        <v>1.310000000000001</v>
       </c>
       <c r="G3">
-        <v>2.030000000000001</v>
+        <v>1.310000000000001</v>
       </c>
       <c r="H3">
         <v>2.030000000000001</v>
@@ -36970,43 +37615,43 @@
         <v>2.030000000000001</v>
       </c>
       <c r="M3">
+        <v>2.030000000000001</v>
+      </c>
+      <c r="N3">
+        <v>2.030000000000001</v>
+      </c>
+      <c r="O3">
+        <v>2.030000000000001</v>
+      </c>
+      <c r="P3">
+        <v>2.030000000000001</v>
+      </c>
+      <c r="Q3">
+        <v>2.030000000000001</v>
+      </c>
+      <c r="R3">
+        <v>2.030000000000001</v>
+      </c>
+      <c r="S3">
+        <v>2.030000000000001</v>
+      </c>
+      <c r="T3">
+        <v>2.030000000000001</v>
+      </c>
+      <c r="U3">
         <v>0.6800000000000004</v>
       </c>
-      <c r="N3">
+      <c r="V3">
         <v>0.6800000000000004</v>
       </c>
-      <c r="O3">
+      <c r="W3">
         <v>0.6800000000000004</v>
       </c>
-      <c r="P3">
+      <c r="X3">
         <v>0.6800000000000004</v>
       </c>
-      <c r="Q3">
+      <c r="Y3">
         <v>0.6700000000000004</v>
-      </c>
-      <c r="R3">
-        <v>2.719999999999986</v>
-      </c>
-      <c r="S3">
-        <v>2.719999999999986</v>
-      </c>
-      <c r="T3">
-        <v>2.719999999999986</v>
-      </c>
-      <c r="U3">
-        <v>2.719999999999986</v>
-      </c>
-      <c r="V3">
-        <v>2.719999999999986</v>
-      </c>
-      <c r="W3">
-        <v>2.719999999999986</v>
-      </c>
-      <c r="X3">
-        <v>2.719999999999986</v>
-      </c>
-      <c r="Y3">
-        <v>2.719999999999986</v>
       </c>
       <c r="Z3">
         <v>2.719999999999986</v>
@@ -37108,268 +37753,484 @@
         <v>2.719999999999986</v>
       </c>
       <c r="BG3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="BH3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="BI3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="BJ3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="BK3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="BL3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="BM3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="BN3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="BO3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="BP3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="BQ3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="BR3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="BS3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="BT3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="BU3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="BV3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="BW3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="BX3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="BY3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="BZ3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="CA3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="CB3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="CC3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="CD3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="CE3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="CF3">
+        <v>2.719999999999986</v>
+      </c>
+      <c r="CG3">
         <v>1.360000000000001</v>
       </c>
-      <c r="BH3">
+      <c r="CH3">
         <v>1.360000000000001</v>
       </c>
-      <c r="BI3">
+      <c r="CI3">
         <v>1.360000000000001</v>
       </c>
-      <c r="BJ3">
+      <c r="CJ3">
         <v>1.360000000000001</v>
       </c>
-      <c r="BK3">
+      <c r="CK3">
         <v>1.360000000000001</v>
       </c>
-      <c r="BL3">
+      <c r="CL3">
+        <v>1.360000000000001</v>
+      </c>
+      <c r="CM3">
+        <v>1.360000000000001</v>
+      </c>
+      <c r="CN3">
+        <v>1.360000000000001</v>
+      </c>
+      <c r="CO3">
+        <v>1.360000000000001</v>
+      </c>
+      <c r="CP3">
+        <v>1.360000000000001</v>
+      </c>
+      <c r="CQ3">
         <v>0.6700000000000004</v>
       </c>
-      <c r="BM3">
+      <c r="CR3">
         <v>0.6700000000000004</v>
       </c>
-      <c r="BN3">
+      <c r="CS3">
         <v>0.6700000000000004</v>
       </c>
-      <c r="BO3">
+      <c r="CT3">
         <v>0.6700000000000004</v>
       </c>
-      <c r="BP3">
+      <c r="CU3">
         <v>0.6700000000000004</v>
       </c>
-      <c r="BQ3">
+      <c r="CV3">
         <v>0.6700000000000004</v>
       </c>
-      <c r="BR3">
+      <c r="CW3">
         <v>0.6700000000000004</v>
       </c>
-      <c r="BS3">
+      <c r="CX3">
         <v>0.6700000000000004</v>
       </c>
-      <c r="BT3">
+      <c r="CY3">
         <v>0.6700000000000004</v>
       </c>
-      <c r="BU3">
+      <c r="CZ3">
         <v>0.6700000000000004</v>
       </c>
-      <c r="BV3">
+      <c r="DA3">
         <v>0.6700000000000004</v>
       </c>
-      <c r="BW3">
+      <c r="DB3">
         <v>0.6700000000000004</v>
       </c>
-      <c r="BX3">
+      <c r="DC3">
         <v>0.6700000000000004</v>
       </c>
-      <c r="BY3">
+      <c r="DD3">
         <v>0.6700000000000004</v>
       </c>
-      <c r="BZ3">
+      <c r="DE3">
         <v>0.6700000000000004</v>
       </c>
-      <c r="CA3">
+      <c r="DF3">
         <v>0.6700000000000004</v>
       </c>
-      <c r="CB3">
+      <c r="DG3">
         <v>0.6700000000000004</v>
       </c>
-      <c r="CC3">
+      <c r="DH3">
         <v>0.6700000000000004</v>
       </c>
-      <c r="CD3">
+      <c r="DI3">
         <v>0.6700000000000004</v>
       </c>
-      <c r="CE3">
+      <c r="DJ3">
         <v>0.6700000000000004</v>
       </c>
-      <c r="CF3">
+      <c r="DK3">
         <v>0.6700000000000004</v>
       </c>
-      <c r="CG3">
+      <c r="DL3">
+        <v>0.6700000000000004</v>
+      </c>
+      <c r="DM3">
+        <v>0.6700000000000004</v>
+      </c>
+      <c r="DN3">
+        <v>0.6700000000000004</v>
+      </c>
+      <c r="DO3">
+        <v>0.6700000000000004</v>
+      </c>
+      <c r="DP3">
+        <v>0.6700000000000004</v>
+      </c>
+      <c r="DQ3">
+        <v>0.6700000000000004</v>
+      </c>
+      <c r="DR3">
+        <v>0.6700000000000004</v>
+      </c>
+      <c r="DS3">
+        <v>0.6700000000000004</v>
+      </c>
+      <c r="DT3">
+        <v>0.6700000000000004</v>
+      </c>
+      <c r="DU3">
+        <v>0.6700000000000004</v>
+      </c>
+      <c r="DV3">
+        <v>0.6700000000000004</v>
+      </c>
+      <c r="DW3">
+        <v>0.6700000000000004</v>
+      </c>
+      <c r="DX3">
+        <v>0.6700000000000004</v>
+      </c>
+      <c r="DY3">
+        <v>0.6700000000000004</v>
+      </c>
+      <c r="DZ3">
+        <v>0.6700000000000004</v>
+      </c>
+      <c r="EA3">
+        <v>0.6700000000000004</v>
+      </c>
+      <c r="EB3">
         <v>2.08</v>
       </c>
-      <c r="CH3">
+      <c r="EC3">
         <v>2.08</v>
       </c>
-      <c r="CI3">
+      <c r="ED3">
         <v>2.08</v>
       </c>
-      <c r="CJ3">
+      <c r="EE3">
         <v>2.08</v>
       </c>
-      <c r="CK3">
+      <c r="EF3">
         <v>2.08</v>
       </c>
-      <c r="CL3">
+      <c r="EG3">
         <v>2.08</v>
       </c>
-      <c r="CM3">
+      <c r="EH3">
         <v>2.08</v>
       </c>
-      <c r="CN3">
+      <c r="EI3">
         <v>2.08</v>
       </c>
-      <c r="CO3">
+      <c r="EJ3">
         <v>2.08</v>
       </c>
-      <c r="CP3">
+      <c r="EK3">
         <v>2.08</v>
       </c>
-      <c r="CQ3">
+      <c r="EL3">
         <v>2.08</v>
       </c>
-      <c r="CR3">
+      <c r="EM3">
         <v>2.08</v>
       </c>
-      <c r="CS3">
+      <c r="EN3">
         <v>2.08</v>
       </c>
-      <c r="CT3">
+      <c r="EO3">
         <v>2.08</v>
       </c>
-      <c r="CU3">
+      <c r="EP3">
         <v>2.08</v>
       </c>
-      <c r="CV3">
+      <c r="EQ3">
         <v>2.08</v>
       </c>
-      <c r="CW3">
+      <c r="ER3">
         <v>2.08</v>
       </c>
-      <c r="CX3">
+      <c r="ES3">
         <v>2.08</v>
       </c>
-      <c r="CY3">
+      <c r="ET3">
         <v>2.08</v>
       </c>
-      <c r="CZ3">
+      <c r="EU3">
         <v>2.08</v>
       </c>
-      <c r="DA3">
+      <c r="EV3">
         <v>2.08</v>
       </c>
-      <c r="DB3">
+      <c r="EW3">
         <v>2.08</v>
       </c>
-      <c r="DC3">
+      <c r="EX3">
         <v>2.08</v>
       </c>
-      <c r="DD3">
+      <c r="EY3">
         <v>2.08</v>
       </c>
-      <c r="DE3">
+      <c r="EZ3">
         <v>2.08</v>
       </c>
-      <c r="DF3">
+      <c r="FA3">
         <v>2.08</v>
       </c>
-      <c r="DG3">
+      <c r="FB3">
         <v>2.08</v>
       </c>
-      <c r="DH3">
+      <c r="FC3">
         <v>2.08</v>
       </c>
-      <c r="DI3">
+      <c r="FD3">
         <v>2.08</v>
       </c>
-      <c r="DJ3">
+      <c r="FE3">
         <v>2.08</v>
       </c>
-      <c r="DK3">
+      <c r="FF3">
         <v>2.08</v>
       </c>
-      <c r="DL3">
+      <c r="FG3">
         <v>2.08</v>
       </c>
-      <c r="DM3">
+      <c r="FH3">
         <v>2.08</v>
       </c>
-      <c r="DN3">
+      <c r="FI3">
         <v>2.08</v>
       </c>
-      <c r="DO3">
+      <c r="FJ3">
         <v>2.08</v>
       </c>
-      <c r="DP3">
+      <c r="FK3">
         <v>2.08</v>
       </c>
-      <c r="DQ3">
+      <c r="FL3">
         <v>2.08</v>
       </c>
-      <c r="DR3">
+      <c r="FM3">
         <v>2.08</v>
       </c>
-      <c r="DS3">
+      <c r="FN3">
         <v>2.08</v>
       </c>
-      <c r="DT3">
+      <c r="FO3">
+        <v>2.08</v>
+      </c>
+      <c r="FP3">
+        <v>2.08</v>
+      </c>
+      <c r="FQ3">
+        <v>2.08</v>
+      </c>
+      <c r="FR3">
+        <v>2.08</v>
+      </c>
+      <c r="FS3">
+        <v>2.08</v>
+      </c>
+      <c r="FT3">
+        <v>2.08</v>
+      </c>
+      <c r="FU3">
+        <v>2.08</v>
+      </c>
+      <c r="FV3">
+        <v>2.08</v>
+      </c>
+      <c r="FW3">
+        <v>2.08</v>
+      </c>
+      <c r="FX3">
+        <v>2.08</v>
+      </c>
+      <c r="FY3">
+        <v>2.08</v>
+      </c>
+      <c r="FZ3">
+        <v>2.08</v>
+      </c>
+      <c r="GA3">
+        <v>2.08</v>
+      </c>
+      <c r="GB3">
+        <v>2.08</v>
+      </c>
+      <c r="GC3">
         <v>2.010000000000001</v>
       </c>
-      <c r="DU3">
+      <c r="GD3">
         <v>2.010000000000001</v>
       </c>
-      <c r="DV3">
+      <c r="GE3">
         <v>2.010000000000001</v>
       </c>
-      <c r="DW3">
+      <c r="GF3">
         <v>2.010000000000001</v>
       </c>
-      <c r="DX3">
+      <c r="GG3">
         <v>2.010000000000001</v>
       </c>
-      <c r="DY3">
+      <c r="GH3">
+        <v>2.010000000000001</v>
+      </c>
+      <c r="GI3">
+        <v>2.010000000000001</v>
+      </c>
+      <c r="GJ3">
+        <v>2.010000000000001</v>
+      </c>
+      <c r="GK3">
         <v>2.000000000000001</v>
       </c>
-      <c r="DZ3">
+      <c r="GL3">
         <v>2.000000000000001</v>
       </c>
-      <c r="EA3">
-        <v>2.000000000000001</v>
-      </c>
-      <c r="EB3">
-        <v>2.000000000000001</v>
-      </c>
-      <c r="EC3">
+      <c r="GM3">
         <v>0.6600000000000004</v>
       </c>
-      <c r="ED3">
+      <c r="GN3">
         <v>0.6600000000000004</v>
       </c>
-      <c r="EE3">
+      <c r="GO3">
         <v>0.6600000000000004</v>
       </c>
-      <c r="EF3">
+      <c r="GP3">
         <v>0.6600000000000004</v>
       </c>
-      <c r="EG3">
+      <c r="GQ3">
         <v>0.6600000000000004</v>
       </c>
-      <c r="EH3">
+      <c r="GR3">
         <v>0.6600000000000004</v>
       </c>
-      <c r="EI3">
+      <c r="GS3">
         <v>0.6600000000000004</v>
       </c>
-      <c r="EJ3">
+      <c r="GT3">
         <v>0.6600000000000004</v>
       </c>
-      <c r="EK3">
+      <c r="GU3">
         <v>0.6600000000000004</v>
       </c>
-      <c r="EL3">
+      <c r="GV3">
         <v>0.6600000000000004</v>
       </c>
-      <c r="EM3">
+      <c r="GW3">
         <v>0.6600000000000004</v>
       </c>
-      <c r="EN3">
+      <c r="GX3">
         <v>0.6600000000000004</v>
       </c>
-      <c r="EO3">
+      <c r="GY3">
         <v>0.6600000000000004</v>
       </c>
-    </row>
-    <row r="4" spans="1:145">
+      <c r="GZ3">
+        <v>0.6600000000000004</v>
+      </c>
+      <c r="HA3">
+        <v>0.6600000000000004</v>
+      </c>
+      <c r="HB3">
+        <v>0.6600000000000004</v>
+      </c>
+      <c r="HC3">
+        <v>0.6600000000000004</v>
+      </c>
+      <c r="HD3">
+        <v>0.6600000000000004</v>
+      </c>
+      <c r="HE3">
+        <v>0.6600000000000004</v>
+      </c>
+      <c r="HF3">
+        <v>0.6600000000000004</v>
+      </c>
+      <c r="HG3">
+        <v>0.6600000000000004</v>
+      </c>
+      <c r="HH3">
+        <v>0.6600000000000004</v>
+      </c>
+      <c r="HI3">
+        <v>0.6600000000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:217">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -37380,112 +38241,112 @@
         <v>6.718412510414964</v>
       </c>
       <c r="D4">
+        <v>6.718412510414964</v>
+      </c>
+      <c r="E4">
+        <v>6.718412510414964</v>
+      </c>
+      <c r="F4">
         <v>6.7089736737571</v>
       </c>
-      <c r="E4">
+      <c r="G4">
+        <v>6.7089736737571</v>
+      </c>
+      <c r="H4">
         <v>3.941502508049325</v>
       </c>
-      <c r="F4">
+      <c r="I4">
+        <v>3.941502508049325</v>
+      </c>
+      <c r="J4">
         <v>3.941502508048643</v>
       </c>
-      <c r="G4">
+      <c r="K4">
         <v>3.941502508048643</v>
       </c>
-      <c r="H4">
+      <c r="L4">
         <v>3.941502508048643</v>
       </c>
-      <c r="I4">
+      <c r="M4">
         <v>3.941502508048643</v>
       </c>
-      <c r="J4">
+      <c r="N4">
         <v>3.941502508048416</v>
       </c>
-      <c r="K4">
+      <c r="O4">
+        <v>3.941502508048416</v>
+      </c>
+      <c r="P4">
+        <v>3.941502508048416</v>
+      </c>
+      <c r="Q4">
+        <v>3.941502508048416</v>
+      </c>
+      <c r="R4">
         <v>3.933209944208556</v>
       </c>
-      <c r="L4">
+      <c r="S4">
         <v>3.933209944208329</v>
       </c>
-      <c r="M4">
+      <c r="T4">
+        <v>3.933209944208329</v>
+      </c>
+      <c r="U4">
         <v>8.620160216306203</v>
       </c>
-      <c r="N4">
+      <c r="V4">
         <v>8.620160216306203</v>
       </c>
-      <c r="O4">
+      <c r="W4">
         <v>8.620160216306203</v>
       </c>
-      <c r="P4">
+      <c r="X4">
         <v>8.620160216306203</v>
       </c>
-      <c r="Q4">
+      <c r="Y4">
         <v>8.689705333281609</v>
       </c>
-      <c r="R4">
+      <c r="Z4">
         <v>1.960438712822906</v>
       </c>
-      <c r="S4">
+      <c r="AA4">
         <v>1.960438712822906</v>
       </c>
-      <c r="T4">
+      <c r="AB4">
         <v>1.960438712822906</v>
       </c>
-      <c r="U4">
+      <c r="AC4">
         <v>1.960438712822906</v>
       </c>
-      <c r="V4">
+      <c r="AD4">
         <v>1.960438712822906</v>
       </c>
-      <c r="W4">
+      <c r="AE4">
         <v>1.960438712822906</v>
       </c>
-      <c r="X4">
+      <c r="AF4">
         <v>1.960438712822906</v>
       </c>
-      <c r="Y4">
+      <c r="AG4">
+        <v>1.960438712822906</v>
+      </c>
+      <c r="AH4">
+        <v>1.960438712822906</v>
+      </c>
+      <c r="AI4">
+        <v>1.960438712822906</v>
+      </c>
+      <c r="AJ4">
         <v>1.960438712822452</v>
       </c>
-      <c r="Z4">
+      <c r="AK4">
         <v>1.960438712822452</v>
       </c>
-      <c r="AA4">
+      <c r="AL4">
         <v>1.960438712822452</v>
       </c>
-      <c r="AB4">
+      <c r="AM4">
         <v>1.960438712822452</v>
-      </c>
-      <c r="AC4">
-        <v>1.960438712821997</v>
-      </c>
-      <c r="AD4">
-        <v>1.960438712821997</v>
-      </c>
-      <c r="AE4">
-        <v>1.960438712821997</v>
-      </c>
-      <c r="AF4">
-        <v>1.960438712821997</v>
-      </c>
-      <c r="AG4">
-        <v>1.960438712821997</v>
-      </c>
-      <c r="AH4">
-        <v>1.960438712821997</v>
-      </c>
-      <c r="AI4">
-        <v>1.960438712821997</v>
-      </c>
-      <c r="AJ4">
-        <v>1.960438712821997</v>
-      </c>
-      <c r="AK4">
-        <v>1.960438712821997</v>
-      </c>
-      <c r="AL4">
-        <v>1.960438712821997</v>
-      </c>
-      <c r="AM4">
-        <v>1.960438712821997</v>
       </c>
       <c r="AN4">
         <v>1.960438712821997</v>
@@ -37524,285 +38385,501 @@
         <v>1.960438712821997</v>
       </c>
       <c r="AZ4">
+        <v>1.960438712821997</v>
+      </c>
+      <c r="BA4">
+        <v>1.960438712821997</v>
+      </c>
+      <c r="BB4">
+        <v>1.960438712821997</v>
+      </c>
+      <c r="BC4">
+        <v>1.960438712821997</v>
+      </c>
+      <c r="BD4">
+        <v>1.960438712821997</v>
+      </c>
+      <c r="BE4">
+        <v>1.960438712821997</v>
+      </c>
+      <c r="BF4">
+        <v>1.960438712821997</v>
+      </c>
+      <c r="BG4">
+        <v>1.960438712821997</v>
+      </c>
+      <c r="BH4">
+        <v>1.960438712821997</v>
+      </c>
+      <c r="BI4">
+        <v>1.960438712821997</v>
+      </c>
+      <c r="BJ4">
+        <v>1.960438712821997</v>
+      </c>
+      <c r="BK4">
+        <v>1.960438712821997</v>
+      </c>
+      <c r="BL4">
+        <v>1.960438712821997</v>
+      </c>
+      <c r="BM4">
+        <v>1.960438712821997</v>
+      </c>
+      <c r="BN4">
+        <v>1.960438712821997</v>
+      </c>
+      <c r="BO4">
         <v>1.958965761378749</v>
       </c>
-      <c r="BA4">
+      <c r="BP4">
         <v>1.958965761378749</v>
       </c>
-      <c r="BB4">
+      <c r="BQ4">
         <v>1.958965761378749</v>
       </c>
-      <c r="BC4">
+      <c r="BR4">
+        <v>1.958965761378749</v>
+      </c>
+      <c r="BS4">
         <v>1.958965761378295</v>
       </c>
-      <c r="BD4">
+      <c r="BT4">
+        <v>1.958965761378295</v>
+      </c>
+      <c r="BU4">
+        <v>1.958965761378295</v>
+      </c>
+      <c r="BV4">
+        <v>1.958965761378295</v>
+      </c>
+      <c r="BW4">
+        <v>1.958965761378295</v>
+      </c>
+      <c r="BX4">
         <v>1.95896576137784</v>
       </c>
-      <c r="BE4">
+      <c r="BY4">
         <v>1.95896576137784</v>
       </c>
-      <c r="BF4">
+      <c r="BZ4">
         <v>1.95896576137784</v>
       </c>
-      <c r="BG4">
+      <c r="CA4">
+        <v>1.95896576137784</v>
+      </c>
+      <c r="CB4">
+        <v>1.95896576137784</v>
+      </c>
+      <c r="CC4">
+        <v>1.95896576137784</v>
+      </c>
+      <c r="CD4">
+        <v>1.95896576137784</v>
+      </c>
+      <c r="CE4">
+        <v>1.95896576137784</v>
+      </c>
+      <c r="CF4">
+        <v>1.95896576137784</v>
+      </c>
+      <c r="CG4">
         <v>3.917879418341272</v>
       </c>
-      <c r="BH4">
+      <c r="CH4">
         <v>3.917879418341272</v>
       </c>
-      <c r="BI4">
+      <c r="CI4">
+        <v>3.917879418341272</v>
+      </c>
+      <c r="CJ4">
+        <v>3.917879418341272</v>
+      </c>
+      <c r="CK4">
         <v>3.917879418340817</v>
       </c>
-      <c r="BJ4">
+      <c r="CL4">
         <v>3.917879418340817</v>
       </c>
-      <c r="BK4">
+      <c r="CM4">
         <v>3.917879418340817</v>
       </c>
-      <c r="BL4">
+      <c r="CN4">
+        <v>3.917879418340817</v>
+      </c>
+      <c r="CO4">
+        <v>3.917879418340817</v>
+      </c>
+      <c r="CP4">
+        <v>3.917879418340817</v>
+      </c>
+      <c r="CQ4">
         <v>6.768584142669852</v>
       </c>
-      <c r="BM4">
+      <c r="CR4">
         <v>6.768584142669852</v>
       </c>
-      <c r="BN4">
+      <c r="CS4">
         <v>6.768584142669852</v>
       </c>
-      <c r="BO4">
+      <c r="CT4">
+        <v>6.768584142669852</v>
+      </c>
+      <c r="CU4">
+        <v>6.752576410624215</v>
+      </c>
+      <c r="CV4">
+        <v>6.752576410624215</v>
+      </c>
+      <c r="CW4">
+        <v>6.752576410624215</v>
+      </c>
+      <c r="CX4">
+        <v>6.752576410624215</v>
+      </c>
+      <c r="CY4">
         <v>6.740517037362451</v>
       </c>
-      <c r="BP4">
+      <c r="CZ4">
         <v>6.740517037362451</v>
       </c>
-      <c r="BQ4">
+      <c r="DA4">
         <v>6.740517037362451</v>
       </c>
-      <c r="BR4">
+      <c r="DB4">
         <v>6.740517037361997</v>
       </c>
-      <c r="BS4">
+      <c r="DC4">
+        <v>6.740517037361997</v>
+      </c>
+      <c r="DD4">
         <v>6.740514209037656</v>
       </c>
-      <c r="BT4">
+      <c r="DE4">
         <v>6.740514209037656</v>
       </c>
-      <c r="BU4">
+      <c r="DF4">
+        <v>6.740514209037656</v>
+      </c>
+      <c r="DG4">
+        <v>6.740514209037656</v>
+      </c>
+      <c r="DH4">
+        <v>6.740514209037656</v>
+      </c>
+      <c r="DI4">
+        <v>6.740514209037656</v>
+      </c>
+      <c r="DJ4">
+        <v>6.740514209037656</v>
+      </c>
+      <c r="DK4">
+        <v>6.740514209037656</v>
+      </c>
+      <c r="DL4">
+        <v>6.740514209037656</v>
+      </c>
+      <c r="DM4">
+        <v>6.740514209037656</v>
+      </c>
+      <c r="DN4">
         <v>6.68970462539346</v>
       </c>
-      <c r="BV4">
+      <c r="DO4">
         <v>6.68970462539346</v>
       </c>
-      <c r="BW4">
+      <c r="DP4">
         <v>6.68970462539346</v>
       </c>
-      <c r="BX4">
+      <c r="DQ4">
+        <v>6.68970462539346</v>
+      </c>
+      <c r="DR4">
+        <v>6.68970462539346</v>
+      </c>
+      <c r="DS4">
         <v>6.689701697053124</v>
       </c>
-      <c r="BY4">
+      <c r="DT4">
         <v>6.689701697053124</v>
       </c>
-      <c r="BZ4">
+      <c r="DU4">
         <v>6.689701697053124</v>
       </c>
-      <c r="CA4">
+      <c r="DV4">
         <v>6.689701697053124</v>
       </c>
-      <c r="CB4">
+      <c r="DW4">
         <v>6.689701697053124</v>
       </c>
-      <c r="CC4">
+      <c r="DX4">
         <v>6.689701697053124</v>
       </c>
-      <c r="CD4">
+      <c r="DY4">
         <v>6.689701697052897</v>
       </c>
-      <c r="CE4">
+      <c r="DZ4">
         <v>6.689701697052897</v>
       </c>
-      <c r="CF4">
+      <c r="EA4">
         <v>6.689701697052897</v>
       </c>
-      <c r="CG4">
+      <c r="EB4">
         <v>1.975086749121601</v>
       </c>
-      <c r="CH4">
+      <c r="EC4">
         <v>1.975086749121601</v>
       </c>
-      <c r="CI4">
+      <c r="ED4">
         <v>1.975086749121601</v>
       </c>
-      <c r="CJ4">
+      <c r="EE4">
         <v>1.975086749121601</v>
       </c>
-      <c r="CK4">
+      <c r="EF4">
         <v>1.975086749121601</v>
       </c>
-      <c r="CL4">
+      <c r="EG4">
         <v>1.975086749121601</v>
       </c>
-      <c r="CM4">
+      <c r="EH4">
         <v>1.975086749121601</v>
       </c>
-      <c r="CN4">
+      <c r="EI4">
         <v>1.975086749121601</v>
       </c>
-      <c r="CO4">
+      <c r="EJ4">
         <v>1.975086749121147</v>
       </c>
-      <c r="CP4">
+      <c r="EK4">
         <v>1.975086749121147</v>
       </c>
-      <c r="CQ4">
+      <c r="EL4">
         <v>1.975086749121147</v>
       </c>
-      <c r="CR4">
+      <c r="EM4">
         <v>1.975086749121147</v>
       </c>
-      <c r="CS4">
+      <c r="EN4">
         <v>1.975086749121147</v>
       </c>
-      <c r="CT4">
+      <c r="EO4">
         <v>1.975086749121147</v>
       </c>
-      <c r="CU4">
+      <c r="EP4">
         <v>1.975086749121147</v>
       </c>
-      <c r="CV4">
+      <c r="EQ4">
         <v>1.975086749121147</v>
       </c>
-      <c r="CW4">
+      <c r="ER4">
         <v>1.975086749121147</v>
       </c>
-      <c r="CX4">
+      <c r="ES4">
         <v>1.975086749121147</v>
       </c>
-      <c r="CY4">
+      <c r="ET4">
         <v>1.975086749121147</v>
       </c>
-      <c r="CZ4">
+      <c r="EU4">
         <v>1.975086749121147</v>
       </c>
-      <c r="DA4">
+      <c r="EV4">
         <v>1.975086749121147</v>
       </c>
-      <c r="DB4">
+      <c r="EW4">
         <v>1.975086749121147</v>
       </c>
-      <c r="DC4">
+      <c r="EX4">
         <v>1.975086749121147</v>
       </c>
-      <c r="DD4">
+      <c r="EY4">
+        <v>1.975086749121147</v>
+      </c>
+      <c r="EZ4">
+        <v>1.975086749121147</v>
+      </c>
+      <c r="FA4">
+        <v>1.975086749121147</v>
+      </c>
+      <c r="FB4">
+        <v>1.975086749121147</v>
+      </c>
+      <c r="FC4">
+        <v>1.975086749121147</v>
+      </c>
+      <c r="FD4">
+        <v>1.975086749121147</v>
+      </c>
+      <c r="FE4">
+        <v>1.975086749121147</v>
+      </c>
+      <c r="FF4">
+        <v>1.975086749121147</v>
+      </c>
+      <c r="FG4">
         <v>1.975086749120692</v>
       </c>
-      <c r="DE4">
+      <c r="FH4">
         <v>1.975086749120692</v>
       </c>
-      <c r="DF4">
+      <c r="FI4">
         <v>1.975086749120692</v>
       </c>
-      <c r="DG4">
+      <c r="FJ4">
         <v>1.975086749120692</v>
       </c>
-      <c r="DH4">
+      <c r="FK4">
         <v>1.973195708863386</v>
       </c>
-      <c r="DI4">
+      <c r="FL4">
         <v>1.973195708863386</v>
       </c>
-      <c r="DJ4">
+      <c r="FM4">
         <v>1.973195708863386</v>
       </c>
-      <c r="DK4">
+      <c r="FN4">
         <v>1.973195708863386</v>
       </c>
-      <c r="DL4">
+      <c r="FO4">
         <v>1.973195708863386</v>
       </c>
-      <c r="DM4">
+      <c r="FP4">
         <v>1.973195708863386</v>
       </c>
-      <c r="DN4">
+      <c r="FQ4">
         <v>1.973195708863386</v>
       </c>
-      <c r="DO4">
+      <c r="FR4">
         <v>1.973195708863386</v>
       </c>
-      <c r="DP4">
+      <c r="FS4">
         <v>1.973195708863386</v>
       </c>
-      <c r="DQ4">
+      <c r="FT4">
+        <v>1.973195708863386</v>
+      </c>
+      <c r="FU4">
+        <v>1.973195708863386</v>
+      </c>
+      <c r="FV4">
+        <v>1.973195708863386</v>
+      </c>
+      <c r="FW4">
+        <v>1.973195708863386</v>
+      </c>
+      <c r="FX4">
+        <v>1.973195708863386</v>
+      </c>
+      <c r="FY4">
         <v>1.973195708862931</v>
       </c>
-      <c r="DR4">
-        <v>1.973195708862931</v>
-      </c>
-      <c r="DS4">
+      <c r="FZ4">
         <v>1.973195708862477</v>
       </c>
-      <c r="DT4">
+      <c r="GA4">
+        <v>1.973195708862477</v>
+      </c>
+      <c r="GB4">
+        <v>1.973195708862477</v>
+      </c>
+      <c r="GC4">
         <v>1.944212153974377</v>
       </c>
-      <c r="DU4">
+      <c r="GD4">
         <v>1.944212153974377</v>
       </c>
-      <c r="DV4">
+      <c r="GE4">
         <v>1.944212153974377</v>
       </c>
-      <c r="DW4">
+      <c r="GF4">
         <v>1.944212153974377</v>
       </c>
-      <c r="DX4">
+      <c r="GG4">
         <v>1.944212153973695</v>
       </c>
-      <c r="DY4">
+      <c r="GH4">
+        <v>1.944212153973695</v>
+      </c>
+      <c r="GI4">
+        <v>1.944212153973695</v>
+      </c>
+      <c r="GJ4">
+        <v>1.944212153973695</v>
+      </c>
+      <c r="GK4">
         <v>1.952089136819041</v>
       </c>
-      <c r="DZ4">
-        <v>1.952089136819041</v>
-      </c>
-      <c r="EA4">
+      <c r="GL4">
         <v>1.952089136818586</v>
       </c>
-      <c r="EB4">
-        <v>1.952089136818586</v>
-      </c>
-      <c r="EC4">
+      <c r="GM4">
         <v>3.842115817237755</v>
       </c>
-      <c r="ED4">
+      <c r="GN4">
         <v>3.842115817237755</v>
       </c>
-      <c r="EE4">
+      <c r="GO4">
         <v>3.842115817237755</v>
       </c>
-      <c r="EF4">
+      <c r="GP4">
         <v>3.842115817237755</v>
       </c>
-      <c r="EG4">
+      <c r="GQ4">
         <v>3.842115817237755</v>
       </c>
-      <c r="EH4">
+      <c r="GR4">
         <v>3.842115817237755</v>
       </c>
-      <c r="EI4">
+      <c r="GS4">
         <v>3.842115817237755</v>
       </c>
-      <c r="EJ4">
+      <c r="GT4">
+        <v>3.842115817237755</v>
+      </c>
+      <c r="GU4">
+        <v>3.842115817237755</v>
+      </c>
+      <c r="GV4">
+        <v>3.842115817237755</v>
+      </c>
+      <c r="GW4">
         <v>3.842043057530418</v>
       </c>
-      <c r="EK4">
+      <c r="GX4">
+        <v>3.842043057530418</v>
+      </c>
+      <c r="GY4">
+        <v>3.842043057530418</v>
+      </c>
+      <c r="GZ4">
         <v>3.830677147427423</v>
       </c>
-      <c r="EL4">
+      <c r="HA4">
         <v>3.830677147427423</v>
       </c>
-      <c r="EM4">
+      <c r="HB4">
         <v>3.830677147427423</v>
       </c>
-      <c r="EN4">
+      <c r="HC4">
         <v>3.830677147427423</v>
       </c>
-      <c r="EO4">
+      <c r="HD4">
+        <v>3.830677147427423</v>
+      </c>
+      <c r="HE4">
+        <v>3.830677147427423</v>
+      </c>
+      <c r="HF4">
+        <v>3.830677147427423</v>
+      </c>
+      <c r="HG4">
+        <v>3.830677147427423</v>
+      </c>
+      <c r="HH4">
+        <v>3.830604387793073</v>
+      </c>
+      <c r="HI4">
         <v>3.830604387793073</v>
       </c>
     </row>

</xml_diff>